<commit_message>
update elt for riskman.incident_fact to add new column: site.
</commit_message>
<xml_diff>
--- a/Matrix_Bus/RiskMan Bus Matrix.xlsx
+++ b/Matrix_Bus/RiskMan Bus Matrix.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="757" uniqueCount="261">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="762" uniqueCount="262">
   <si>
     <t>Category</t>
   </si>
@@ -833,6 +833,9 @@
   </si>
   <si>
     <t>customerSite</t>
+  </si>
+  <si>
+    <t>site</t>
   </si>
 </sst>
 </file>
@@ -3066,10 +3069,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:L55"/>
+  <dimension ref="A1:L56"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="A58" sqref="A58"/>
+      <selection activeCell="A56" sqref="A50:K56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4453,6 +4456,31 @@
       </c>
       <c r="J55" s="49"/>
       <c r="K55" s="49"/>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A56" s="48" t="s">
+        <v>261</v>
+      </c>
+      <c r="B56" s="49"/>
+      <c r="C56" s="48" t="s">
+        <v>63</v>
+      </c>
+      <c r="D56" s="50">
+        <v>100</v>
+      </c>
+      <c r="E56" s="49"/>
+      <c r="F56" s="49"/>
+      <c r="G56" s="51" t="s">
+        <v>49</v>
+      </c>
+      <c r="H56" s="49" t="s">
+        <v>50</v>
+      </c>
+      <c r="I56" s="51" t="s">
+        <v>261</v>
+      </c>
+      <c r="J56" s="49"/>
+      <c r="K56" s="49"/>
     </row>
   </sheetData>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
add ChCCUNotif to incident_fact in Riskman.Dev
</commit_message>
<xml_diff>
--- a/Matrix_Bus/RiskMan Bus Matrix.xlsx
+++ b/Matrix_Bus/RiskMan Bus Matrix.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="762" uniqueCount="262">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="769" uniqueCount="265">
   <si>
     <t>Category</t>
   </si>
@@ -837,12 +837,21 @@
   <si>
     <t>site</t>
   </si>
+  <si>
+    <t>ChCCUNotif</t>
+  </si>
+  <si>
+    <t>CAbuse_IFR</t>
+  </si>
+  <si>
+    <t>1= yes, 0= no /  use IncidentsForReview.ID join CAbuse_IFR.[CAbuse_ID]</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -898,6 +907,12 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -919,7 +934,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="24">
+  <borders count="26">
     <border>
       <left/>
       <right/>
@@ -1222,11 +1237,31 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -1338,6 +1373,13 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3069,10 +3111,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:L56"/>
+  <dimension ref="A1:L57"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="A56" sqref="A50:K56"/>
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4481,6 +4523,32 @@
       </c>
       <c r="J56" s="49"/>
       <c r="K56" s="49"/>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A57" s="68" t="s">
+        <v>262</v>
+      </c>
+      <c r="C57" s="48" t="s">
+        <v>63</v>
+      </c>
+      <c r="D57" s="50">
+        <v>3</v>
+      </c>
+      <c r="E57" s="51" t="s">
+        <v>93</v>
+      </c>
+      <c r="G57" s="51" t="s">
+        <v>49</v>
+      </c>
+      <c r="H57" t="s">
+        <v>263</v>
+      </c>
+      <c r="I57" s="69" t="s">
+        <v>262</v>
+      </c>
+      <c r="K57" s="70" t="s">
+        <v>264</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update riskman bus matrix to add ContributingFactors_fact
</commit_message>
<xml_diff>
--- a/Matrix_Bus/RiskMan Bus Matrix.xlsx
+++ b/Matrix_Bus/RiskMan Bus Matrix.xlsx
@@ -4,29 +4,30 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="6990" windowWidth="28800" windowHeight="5985" activeTab="1"/>
+    <workbookView xWindow="-90" yWindow="6990" windowWidth="28800" windowHeight="5985" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Bus Matrix" sheetId="1" r:id="rId1"/>
     <sheet name="incident_fact" sheetId="2" r:id="rId2"/>
-    <sheet name="incident_history_fact" sheetId="17" r:id="rId3"/>
-    <sheet name="person_dim" sheetId="6" r:id="rId4"/>
-    <sheet name="Employee_DIM" sheetId="5" r:id="rId5"/>
-    <sheet name="Date_DIM" sheetId="7" r:id="rId6"/>
-    <sheet name="Portfolio_DIM" sheetId="9" r:id="rId7"/>
-    <sheet name="Service_Stream_DIM" sheetId="10" r:id="rId8"/>
-    <sheet name="Program_DIM" sheetId="11" r:id="rId9"/>
-    <sheet name="Incident_Type_DIM" sheetId="13" r:id="rId10"/>
-    <sheet name="action_dim" sheetId="15" r:id="rId11"/>
-    <sheet name="incident_type_fact" sheetId="14" r:id="rId12"/>
-    <sheet name="incident_action_fact" sheetId="16" r:id="rId13"/>
+    <sheet name="ContributingFactors_fact" sheetId="18" r:id="rId3"/>
+    <sheet name="incident_history_fact" sheetId="17" r:id="rId4"/>
+    <sheet name="person_dim" sheetId="6" r:id="rId5"/>
+    <sheet name="Employee_DIM" sheetId="5" r:id="rId6"/>
+    <sheet name="Date_DIM" sheetId="7" r:id="rId7"/>
+    <sheet name="Portfolio_DIM" sheetId="9" r:id="rId8"/>
+    <sheet name="Service_Stream_DIM" sheetId="10" r:id="rId9"/>
+    <sheet name="Program_DIM" sheetId="11" r:id="rId10"/>
+    <sheet name="Incident_Type_DIM" sheetId="13" r:id="rId11"/>
+    <sheet name="action_dim" sheetId="15" r:id="rId12"/>
+    <sheet name="incident_type_fact" sheetId="14" r:id="rId13"/>
+    <sheet name="incident_action_fact" sheetId="16" r:id="rId14"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="769" uniqueCount="265">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="819" uniqueCount="276">
   <si>
     <t>Category</t>
   </si>
@@ -845,6 +846,49 @@
   </si>
   <si>
     <t>1= yes, 0= no /  use IncidentsForReview.ID join CAbuse_IFR.[CAbuse_ID]</t>
+  </si>
+  <si>
+    <t>ContributingFactors_Fact</t>
+  </si>
+  <si>
+    <t>Used to store contributing factors</t>
+  </si>
+  <si>
+    <t>display_id</t>
+  </si>
+  <si>
+    <t>CFactorGroup</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> CFactor</t>
+  </si>
+  <si>
+    <t>Equipment</t>
+  </si>
+  <si>
+    <t>Equipment failure / fault</t>
+  </si>
+  <si>
+    <t>tblContributingFactors_IFR</t>
+  </si>
+  <si>
+    <t>CFactor</t>
+  </si>
+  <si>
+    <t>DisplayID</t>
+  </si>
+  <si>
+    <t>select a.id,a.DisplayID
+ from extract_riskman.IncidentsForReview as a
+ inner join
+ (
+ select DisplayID,max(sequenceno) as sequenceno
+  from extract_riskman.IncidentsForReview
+  where SubModule='Incidents'
+  group by DisplayID
+  ) as b 
+  on  a.SubModule='Incidents' and a.DisplayID=b.DisplayID
+  and a.SequenceNo=b.sequenceno</t>
   </si>
 </sst>
 </file>
@@ -1261,7 +1305,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -1380,6 +1424,12 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1969,6 +2019,134 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16" style="27" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="44.42578125" style="27" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.28515625" style="27" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.5703125" style="27" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.140625" style="27" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" style="27"/>
+    <col min="7" max="7" width="14" style="27" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.28515625" style="27" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.85546875" style="27" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.5703125" style="27" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="68.28515625" style="27" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A1" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="28" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="30" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="30" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="30" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="27" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="27" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="30" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="33" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" s="33" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="33" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" s="33" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8" s="34" t="s">
+        <v>27</v>
+      </c>
+      <c r="F8" s="33" t="s">
+        <v>29</v>
+      </c>
+      <c r="G8" s="33" t="s">
+        <v>30</v>
+      </c>
+      <c r="H8" s="33" t="s">
+        <v>31</v>
+      </c>
+      <c r="I8" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="J8" s="33" t="s">
+        <v>33</v>
+      </c>
+      <c r="K8" s="33" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="31"/>
+      <c r="B9" s="32"/>
+      <c r="C9" s="32"/>
+      <c r="D9" s="32"/>
+      <c r="E9" s="32"/>
+      <c r="F9" s="32"/>
+      <c r="G9" s="32"/>
+      <c r="H9" s="32"/>
+      <c r="I9" s="32"/>
+      <c r="J9" s="32"/>
+      <c r="K9" s="32"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="32"/>
+      <c r="B10" s="32"/>
+      <c r="C10" s="32"/>
+      <c r="D10" s="32"/>
+      <c r="E10" s="32"/>
+      <c r="F10" s="32"/>
+      <c r="G10" s="32"/>
+      <c r="H10" s="35"/>
+      <c r="I10" s="32"/>
+      <c r="J10" s="32"/>
+      <c r="K10" s="32"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2178,7 +2356,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K19"/>
   <sheetViews>
@@ -2581,7 +2759,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K12"/>
   <sheetViews>
@@ -2844,7 +3022,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K12"/>
   <sheetViews>
@@ -3113,8 +3291,8 @@
   </sheetPr>
   <dimension ref="A1:L57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4557,6 +4735,229 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M10" sqref="M10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.5703125" customWidth="1"/>
+    <col min="2" max="2" width="39.85546875" customWidth="1"/>
+    <col min="5" max="5" width="20.140625" customWidth="1"/>
+    <col min="7" max="7" width="21.85546875" customWidth="1"/>
+    <col min="8" max="8" width="31.28515625" customWidth="1"/>
+    <col min="9" max="9" width="23.28515625" customWidth="1"/>
+    <col min="10" max="10" width="19.7109375" customWidth="1"/>
+    <col min="11" max="11" width="41.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" s="27" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A1" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="28" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="30" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="27" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="27" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="30" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="27" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="27" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="27" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" s="27" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="1:11" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="F8" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="G8" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="H8" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="I8" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="J8" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="K8" s="13" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="71" t="s">
+        <v>135</v>
+      </c>
+      <c r="B9" s="71"/>
+      <c r="C9" s="71" t="s">
+        <v>62</v>
+      </c>
+      <c r="D9" s="71"/>
+      <c r="E9" s="71">
+        <v>44</v>
+      </c>
+      <c r="F9" s="71"/>
+      <c r="G9" s="71" t="s">
+        <v>49</v>
+      </c>
+      <c r="H9" s="71" t="s">
+        <v>272</v>
+      </c>
+      <c r="I9" s="71" t="s">
+        <v>135</v>
+      </c>
+      <c r="J9" s="71" t="s">
+        <v>62</v>
+      </c>
+      <c r="K9" s="71"/>
+    </row>
+    <row r="10" spans="1:11" ht="210" x14ac:dyDescent="0.25">
+      <c r="A10" s="71" t="s">
+        <v>267</v>
+      </c>
+      <c r="B10" s="71"/>
+      <c r="C10" s="71" t="s">
+        <v>62</v>
+      </c>
+      <c r="D10" s="71"/>
+      <c r="E10" s="71">
+        <v>15</v>
+      </c>
+      <c r="F10" s="71"/>
+      <c r="G10" s="71" t="s">
+        <v>49</v>
+      </c>
+      <c r="H10" s="71" t="s">
+        <v>50</v>
+      </c>
+      <c r="I10" s="71" t="s">
+        <v>274</v>
+      </c>
+      <c r="J10" s="71" t="s">
+        <v>62</v>
+      </c>
+      <c r="K10" s="72" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="71" t="s">
+        <v>268</v>
+      </c>
+      <c r="B11" s="71"/>
+      <c r="C11" s="71" t="s">
+        <v>63</v>
+      </c>
+      <c r="D11" s="71">
+        <v>400</v>
+      </c>
+      <c r="E11" s="71" t="s">
+        <v>270</v>
+      </c>
+      <c r="F11" s="71"/>
+      <c r="G11" s="71" t="s">
+        <v>49</v>
+      </c>
+      <c r="H11" s="71" t="s">
+        <v>272</v>
+      </c>
+      <c r="I11" s="71" t="s">
+        <v>268</v>
+      </c>
+      <c r="J11" s="71" t="s">
+        <v>63</v>
+      </c>
+      <c r="K11" s="71"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="71" t="s">
+        <v>269</v>
+      </c>
+      <c r="B12" s="71"/>
+      <c r="C12" s="71" t="s">
+        <v>63</v>
+      </c>
+      <c r="D12" s="71">
+        <v>400</v>
+      </c>
+      <c r="E12" s="71" t="s">
+        <v>271</v>
+      </c>
+      <c r="F12" s="71"/>
+      <c r="G12" s="71" t="s">
+        <v>49</v>
+      </c>
+      <c r="H12" s="71" t="s">
+        <v>272</v>
+      </c>
+      <c r="I12" s="71" t="s">
+        <v>273</v>
+      </c>
+      <c r="J12" s="71" t="s">
+        <v>63</v>
+      </c>
+      <c r="K12" s="71"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K17"/>
   <sheetViews>
@@ -4886,7 +5287,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K14"/>
   <sheetViews>
@@ -5194,7 +5595,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K10"/>
   <sheetViews>
@@ -5378,7 +5779,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K10"/>
   <sheetViews>
@@ -5506,7 +5907,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K10"/>
   <sheetViews>
@@ -5569,134 +5970,6 @@
       </c>
       <c r="B6" s="27" t="s">
         <v>117</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="33" t="s">
-        <v>25</v>
-      </c>
-      <c r="B8" s="33" t="s">
-        <v>20</v>
-      </c>
-      <c r="C8" s="33" t="s">
-        <v>26</v>
-      </c>
-      <c r="D8" s="33" t="s">
-        <v>22</v>
-      </c>
-      <c r="E8" s="34" t="s">
-        <v>27</v>
-      </c>
-      <c r="F8" s="33" t="s">
-        <v>29</v>
-      </c>
-      <c r="G8" s="33" t="s">
-        <v>30</v>
-      </c>
-      <c r="H8" s="33" t="s">
-        <v>31</v>
-      </c>
-      <c r="I8" s="33" t="s">
-        <v>32</v>
-      </c>
-      <c r="J8" s="33" t="s">
-        <v>33</v>
-      </c>
-      <c r="K8" s="33" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="31"/>
-      <c r="B9" s="32"/>
-      <c r="C9" s="32"/>
-      <c r="D9" s="32"/>
-      <c r="E9" s="32"/>
-      <c r="F9" s="32"/>
-      <c r="G9" s="32"/>
-      <c r="H9" s="32"/>
-      <c r="I9" s="32"/>
-      <c r="J9" s="32"/>
-      <c r="K9" s="32"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="32"/>
-      <c r="B10" s="32"/>
-      <c r="C10" s="32"/>
-      <c r="D10" s="32"/>
-      <c r="E10" s="32"/>
-      <c r="F10" s="32"/>
-      <c r="G10" s="32"/>
-      <c r="H10" s="35"/>
-      <c r="I10" s="32"/>
-      <c r="J10" s="32"/>
-      <c r="K10" s="32"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K10"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16" style="27" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="44.42578125" style="27" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.28515625" style="27" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4.5703125" style="27" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.140625" style="27" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" style="27"/>
-    <col min="7" max="7" width="14" style="27" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.28515625" style="27" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.85546875" style="27" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.5703125" style="27" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="68.28515625" style="27" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:11" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="29" t="s">
-        <v>17</v>
-      </c>
-      <c r="B1" s="28" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="30" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="30" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="30" t="s">
-        <v>20</v>
-      </c>
-      <c r="B4" s="27" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="B5" s="27" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="30" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -5793,7 +6066,7 @@
         <v>17</v>
       </c>
       <c r="B1" s="28" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
add etl for riskman.feedback_fact.
</commit_message>
<xml_diff>
--- a/Matrix_Bus/RiskMan Bus Matrix.xlsx
+++ b/Matrix_Bus/RiskMan Bus Matrix.xlsx
@@ -4,30 +4,32 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="6990" windowWidth="28800" windowHeight="5985" activeTab="2"/>
+    <workbookView xWindow="-90" yWindow="7050" windowWidth="24090" windowHeight="3075" firstSheet="8" activeTab="15"/>
   </bookViews>
   <sheets>
     <sheet name="Bus Matrix" sheetId="1" r:id="rId1"/>
     <sheet name="incident_fact" sheetId="2" r:id="rId2"/>
-    <sheet name="ContributingFactors_fact" sheetId="18" r:id="rId3"/>
-    <sheet name="incident_history_fact" sheetId="17" r:id="rId4"/>
-    <sheet name="person_dim" sheetId="6" r:id="rId5"/>
-    <sheet name="Employee_DIM" sheetId="5" r:id="rId6"/>
-    <sheet name="Date_DIM" sheetId="7" r:id="rId7"/>
-    <sheet name="Portfolio_DIM" sheetId="9" r:id="rId8"/>
-    <sheet name="Service_Stream_DIM" sheetId="10" r:id="rId9"/>
-    <sheet name="Program_DIM" sheetId="11" r:id="rId10"/>
-    <sheet name="Incident_Type_DIM" sheetId="13" r:id="rId11"/>
-    <sheet name="action_dim" sheetId="15" r:id="rId12"/>
-    <sheet name="incident_type_fact" sheetId="14" r:id="rId13"/>
-    <sheet name="incident_action_fact" sheetId="16" r:id="rId14"/>
+    <sheet name="feedback_fact" sheetId="19" r:id="rId3"/>
+    <sheet name="Sheet2" sheetId="20" r:id="rId4"/>
+    <sheet name="ContributingFactors_fact" sheetId="18" r:id="rId5"/>
+    <sheet name="incident_history_fact" sheetId="17" r:id="rId6"/>
+    <sheet name="person_dim" sheetId="6" r:id="rId7"/>
+    <sheet name="Employee_DIM" sheetId="5" r:id="rId8"/>
+    <sheet name="Date_DIM" sheetId="7" r:id="rId9"/>
+    <sheet name="Portfolio_DIM" sheetId="9" r:id="rId10"/>
+    <sheet name="Service_Stream_DIM" sheetId="10" r:id="rId11"/>
+    <sheet name="Program_DIM" sheetId="11" r:id="rId12"/>
+    <sheet name="Incident_Type_DIM" sheetId="13" r:id="rId13"/>
+    <sheet name="action_dim" sheetId="15" r:id="rId14"/>
+    <sheet name="incident_type_fact" sheetId="14" r:id="rId15"/>
+    <sheet name="incident_action_fact" sheetId="16" r:id="rId16"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="819" uniqueCount="276">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1155" uniqueCount="281">
   <si>
     <t>Category</t>
   </si>
@@ -889,6 +891,21 @@
   ) as b 
   on  a.SubModule='Incidents' and a.DisplayID=b.DisplayID
   and a.SequenceNo=b.sequenceno</t>
+  </si>
+  <si>
+    <t>Feedback_Fact</t>
+  </si>
+  <si>
+    <t>Feedback Fact</t>
+  </si>
+  <si>
+    <t>Used to store feedbacks for incidents</t>
+  </si>
+  <si>
+    <t>SubModule='RMFeedback'</t>
+  </si>
+  <si>
+    <t>feedback_key</t>
   </si>
 </sst>
 </file>
@@ -1305,7 +1322,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="73">
+  <cellXfs count="92">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -1430,6 +1447,63 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2022,6 +2096,137 @@
   <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16" style="27" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="44.42578125" style="27" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.28515625" style="27" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.5703125" style="27" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.140625" style="27" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" style="27"/>
+    <col min="7" max="7" width="14" style="27" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.28515625" style="27" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.85546875" style="27" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.5703125" style="27" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="68.28515625" style="27" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A1" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="28" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="30" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="30" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="30" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="27" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="27" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="27" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="33" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" s="33" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="33" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" s="33" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8" s="34" t="s">
+        <v>27</v>
+      </c>
+      <c r="F8" s="33" t="s">
+        <v>29</v>
+      </c>
+      <c r="G8" s="33" t="s">
+        <v>30</v>
+      </c>
+      <c r="H8" s="33" t="s">
+        <v>31</v>
+      </c>
+      <c r="I8" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="J8" s="33" t="s">
+        <v>33</v>
+      </c>
+      <c r="K8" s="33" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="31"/>
+      <c r="B9" s="32"/>
+      <c r="C9" s="32"/>
+      <c r="D9" s="32"/>
+      <c r="E9" s="32"/>
+      <c r="F9" s="32"/>
+      <c r="G9" s="32"/>
+      <c r="H9" s="32"/>
+      <c r="I9" s="32"/>
+      <c r="J9" s="32"/>
+      <c r="K9" s="32"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="32"/>
+      <c r="B10" s="32"/>
+      <c r="C10" s="32"/>
+      <c r="D10" s="32"/>
+      <c r="E10" s="32"/>
+      <c r="F10" s="32"/>
+      <c r="G10" s="32"/>
+      <c r="H10" s="35"/>
+      <c r="I10" s="32"/>
+      <c r="J10" s="32"/>
+      <c r="K10" s="32"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -2045,7 +2250,7 @@
         <v>17</v>
       </c>
       <c r="B1" s="28" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -2145,7 +2350,135 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16" style="27" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="44.42578125" style="27" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.28515625" style="27" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.5703125" style="27" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.140625" style="27" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" style="27"/>
+    <col min="7" max="7" width="14" style="27" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.28515625" style="27" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.85546875" style="27" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.5703125" style="27" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="68.28515625" style="27" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A1" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="28" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="30" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="30" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="30" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="27" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="27" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="30" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="33" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" s="33" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="33" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" s="33" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8" s="34" t="s">
+        <v>27</v>
+      </c>
+      <c r="F8" s="33" t="s">
+        <v>29</v>
+      </c>
+      <c r="G8" s="33" t="s">
+        <v>30</v>
+      </c>
+      <c r="H8" s="33" t="s">
+        <v>31</v>
+      </c>
+      <c r="I8" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="J8" s="33" t="s">
+        <v>33</v>
+      </c>
+      <c r="K8" s="33" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="31"/>
+      <c r="B9" s="32"/>
+      <c r="C9" s="32"/>
+      <c r="D9" s="32"/>
+      <c r="E9" s="32"/>
+      <c r="F9" s="32"/>
+      <c r="G9" s="32"/>
+      <c r="H9" s="32"/>
+      <c r="I9" s="32"/>
+      <c r="J9" s="32"/>
+      <c r="K9" s="32"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="32"/>
+      <c r="B10" s="32"/>
+      <c r="C10" s="32"/>
+      <c r="D10" s="32"/>
+      <c r="E10" s="32"/>
+      <c r="F10" s="32"/>
+      <c r="G10" s="32"/>
+      <c r="H10" s="35"/>
+      <c r="I10" s="32"/>
+      <c r="J10" s="32"/>
+      <c r="K10" s="32"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K12"/>
   <sheetViews>
@@ -2356,12 +2689,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:K19"/>
+      <selection activeCell="A16" sqref="A16:XFD16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2759,12 +3092,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3022,12 +3355,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3292,7 +3625,7 @@
   <dimension ref="A1:L57"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD8"/>
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4736,9 +5069,1470 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FFFFFF00"/>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:L57"/>
+  <sheetViews>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="K10" sqref="K10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="38.42578125" style="75" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="64" style="75" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" style="75" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" style="75" customWidth="1"/>
+    <col min="5" max="5" width="12" style="75" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" style="75" customWidth="1"/>
+    <col min="7" max="7" width="14" style="75" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="24" style="75" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="23.7109375" style="75" customWidth="1"/>
+    <col min="10" max="10" width="9.85546875" style="75" customWidth="1"/>
+    <col min="11" max="11" width="67.140625" style="75" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="75"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A1" s="73" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="74" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="76" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="75" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="76" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="75" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="76" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="75" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="76" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="75" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="76" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="75" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="F8" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="G8" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="H8" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="I8" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="J8" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="K8" s="13" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="77" t="s">
+        <v>280</v>
+      </c>
+      <c r="B9" s="71" t="s">
+        <v>48</v>
+      </c>
+      <c r="C9" s="71" t="s">
+        <v>62</v>
+      </c>
+      <c r="D9" s="71"/>
+      <c r="E9" s="71"/>
+      <c r="F9" s="71"/>
+      <c r="G9" s="71"/>
+      <c r="H9" s="71"/>
+      <c r="I9" s="71"/>
+      <c r="J9" s="71"/>
+      <c r="K9" s="72"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="77" t="s">
+        <v>135</v>
+      </c>
+      <c r="B10" s="71" t="s">
+        <v>47</v>
+      </c>
+      <c r="C10" s="71" t="s">
+        <v>62</v>
+      </c>
+      <c r="D10" s="71"/>
+      <c r="E10" s="71"/>
+      <c r="F10" s="71"/>
+      <c r="G10" s="71" t="s">
+        <v>49</v>
+      </c>
+      <c r="H10" s="71" t="s">
+        <v>50</v>
+      </c>
+      <c r="I10" s="71" t="s">
+        <v>46</v>
+      </c>
+      <c r="J10" s="71"/>
+      <c r="K10" s="78" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="B11" s="19" t="s">
+        <v>65</v>
+      </c>
+      <c r="C11" s="71" t="s">
+        <v>62</v>
+      </c>
+      <c r="D11" s="71"/>
+      <c r="E11" s="71"/>
+      <c r="F11" s="71"/>
+      <c r="G11" s="71" t="s">
+        <v>49</v>
+      </c>
+      <c r="H11" s="71" t="s">
+        <v>50</v>
+      </c>
+      <c r="I11" s="71" t="s">
+        <v>88</v>
+      </c>
+      <c r="J11" s="71"/>
+      <c r="K11" s="72" t="s">
+        <v>66</v>
+      </c>
+      <c r="L11" s="79"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" s="77" t="s">
+        <v>136</v>
+      </c>
+      <c r="B12" s="77" t="s">
+        <v>38</v>
+      </c>
+      <c r="C12" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="D12" s="19"/>
+      <c r="E12" s="19"/>
+      <c r="F12" s="71"/>
+      <c r="G12" s="71" t="s">
+        <v>49</v>
+      </c>
+      <c r="H12" s="71" t="s">
+        <v>50</v>
+      </c>
+      <c r="I12" s="71" t="s">
+        <v>6</v>
+      </c>
+      <c r="J12" s="71"/>
+      <c r="K12" s="72" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="B13" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="C13" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="D13" s="21"/>
+      <c r="E13" s="21"/>
+      <c r="F13" s="21"/>
+      <c r="G13" s="71"/>
+      <c r="H13" s="71"/>
+      <c r="I13" s="21"/>
+      <c r="J13" s="21"/>
+      <c r="K13" s="80" t="s">
+        <v>254</v>
+      </c>
+      <c r="L13" s="81"/>
+    </row>
+    <row r="14" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="A14" s="21" t="s">
+        <v>138</v>
+      </c>
+      <c r="B14" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="D14" s="21"/>
+      <c r="E14" s="21"/>
+      <c r="F14" s="21"/>
+      <c r="G14" s="71" t="s">
+        <v>49</v>
+      </c>
+      <c r="H14" s="71" t="s">
+        <v>154</v>
+      </c>
+      <c r="I14" s="21" t="s">
+        <v>253</v>
+      </c>
+      <c r="J14" s="21"/>
+      <c r="K14" s="80" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" s="82" t="s">
+        <v>164</v>
+      </c>
+      <c r="B15" s="71" t="s">
+        <v>37</v>
+      </c>
+      <c r="C15" s="82" t="s">
+        <v>62</v>
+      </c>
+      <c r="D15" s="71"/>
+      <c r="E15" s="71"/>
+      <c r="F15" s="71"/>
+      <c r="G15" s="71" t="s">
+        <v>49</v>
+      </c>
+      <c r="H15" s="71" t="s">
+        <v>50</v>
+      </c>
+      <c r="I15" s="71" t="s">
+        <v>51</v>
+      </c>
+      <c r="J15" s="71"/>
+      <c r="K15" s="72"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" s="82" t="s">
+        <v>52</v>
+      </c>
+      <c r="B16" s="71" t="s">
+        <v>37</v>
+      </c>
+      <c r="C16" s="82" t="s">
+        <v>62</v>
+      </c>
+      <c r="D16" s="71"/>
+      <c r="E16" s="71"/>
+      <c r="F16" s="71"/>
+      <c r="G16" s="71" t="s">
+        <v>49</v>
+      </c>
+      <c r="H16" s="71" t="s">
+        <v>50</v>
+      </c>
+      <c r="I16" s="71" t="s">
+        <v>53</v>
+      </c>
+      <c r="J16" s="71"/>
+      <c r="K16" s="83"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="82" t="s">
+        <v>165</v>
+      </c>
+      <c r="B17" s="71" t="s">
+        <v>37</v>
+      </c>
+      <c r="C17" s="82" t="s">
+        <v>62</v>
+      </c>
+      <c r="D17" s="71"/>
+      <c r="E17" s="71"/>
+      <c r="F17" s="71"/>
+      <c r="G17" s="71" t="s">
+        <v>49</v>
+      </c>
+      <c r="H17" s="71" t="s">
+        <v>50</v>
+      </c>
+      <c r="I17" s="71" t="s">
+        <v>54</v>
+      </c>
+      <c r="J17" s="71"/>
+      <c r="K17" s="72"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="82" t="s">
+        <v>166</v>
+      </c>
+      <c r="B18" s="71" t="s">
+        <v>37</v>
+      </c>
+      <c r="C18" s="82" t="s">
+        <v>62</v>
+      </c>
+      <c r="D18" s="71"/>
+      <c r="E18" s="71"/>
+      <c r="F18" s="71"/>
+      <c r="G18" s="71" t="s">
+        <v>49</v>
+      </c>
+      <c r="H18" s="71" t="s">
+        <v>50</v>
+      </c>
+      <c r="I18" s="71" t="s">
+        <v>60</v>
+      </c>
+      <c r="J18" s="71"/>
+      <c r="K18" s="72"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" s="82" t="s">
+        <v>167</v>
+      </c>
+      <c r="B19" s="71" t="s">
+        <v>37</v>
+      </c>
+      <c r="C19" s="82" t="s">
+        <v>62</v>
+      </c>
+      <c r="D19" s="71"/>
+      <c r="E19" s="71"/>
+      <c r="F19" s="71"/>
+      <c r="G19" s="71" t="s">
+        <v>49</v>
+      </c>
+      <c r="H19" s="71" t="s">
+        <v>154</v>
+      </c>
+      <c r="I19" s="71" t="s">
+        <v>156</v>
+      </c>
+      <c r="J19" s="71"/>
+      <c r="K19" s="72"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" s="82" t="s">
+        <v>168</v>
+      </c>
+      <c r="B20" s="71" t="s">
+        <v>37</v>
+      </c>
+      <c r="C20" s="82" t="s">
+        <v>62</v>
+      </c>
+      <c r="D20" s="71"/>
+      <c r="E20" s="71"/>
+      <c r="F20" s="71"/>
+      <c r="G20" s="71" t="s">
+        <v>49</v>
+      </c>
+      <c r="H20" s="71" t="s">
+        <v>154</v>
+      </c>
+      <c r="I20" s="71" t="s">
+        <v>155</v>
+      </c>
+      <c r="J20" s="71"/>
+      <c r="K20" s="84"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" s="82" t="s">
+        <v>55</v>
+      </c>
+      <c r="B21" s="71"/>
+      <c r="C21" s="82" t="s">
+        <v>64</v>
+      </c>
+      <c r="D21" s="71"/>
+      <c r="E21" s="71"/>
+      <c r="F21" s="71"/>
+      <c r="G21" s="71" t="s">
+        <v>49</v>
+      </c>
+      <c r="H21" s="71" t="s">
+        <v>50</v>
+      </c>
+      <c r="I21" s="71" t="s">
+        <v>56</v>
+      </c>
+      <c r="J21" s="71"/>
+      <c r="K21" s="83"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" s="82" t="s">
+        <v>139</v>
+      </c>
+      <c r="B22" s="71"/>
+      <c r="C22" s="82" t="s">
+        <v>62</v>
+      </c>
+      <c r="D22" s="71"/>
+      <c r="E22" s="71"/>
+      <c r="F22" s="71"/>
+      <c r="G22" s="71" t="s">
+        <v>49</v>
+      </c>
+      <c r="H22" s="71" t="s">
+        <v>50</v>
+      </c>
+      <c r="I22" s="71" t="s">
+        <v>57</v>
+      </c>
+      <c r="J22" s="71"/>
+      <c r="K22" s="72"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" s="82" t="s">
+        <v>140</v>
+      </c>
+      <c r="B23" s="71" t="s">
+        <v>35</v>
+      </c>
+      <c r="C23" s="71" t="s">
+        <v>63</v>
+      </c>
+      <c r="D23" s="71">
+        <v>20</v>
+      </c>
+      <c r="E23" s="71"/>
+      <c r="F23" s="71"/>
+      <c r="G23" s="71" t="s">
+        <v>49</v>
+      </c>
+      <c r="H23" s="71" t="s">
+        <v>50</v>
+      </c>
+      <c r="I23" s="71" t="s">
+        <v>58</v>
+      </c>
+      <c r="J23" s="71"/>
+      <c r="K23" s="72"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" s="71" t="s">
+        <v>141</v>
+      </c>
+      <c r="B24" s="71" t="s">
+        <v>36</v>
+      </c>
+      <c r="C24" s="71" t="s">
+        <v>63</v>
+      </c>
+      <c r="D24" s="71">
+        <v>20</v>
+      </c>
+      <c r="E24" s="71"/>
+      <c r="F24" s="71"/>
+      <c r="G24" s="71" t="s">
+        <v>49</v>
+      </c>
+      <c r="H24" s="71" t="s">
+        <v>50</v>
+      </c>
+      <c r="I24" s="71" t="s">
+        <v>5</v>
+      </c>
+      <c r="J24" s="71"/>
+      <c r="K24" s="71"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" s="82" t="s">
+        <v>142</v>
+      </c>
+      <c r="B25" s="71"/>
+      <c r="C25" s="82" t="s">
+        <v>63</v>
+      </c>
+      <c r="D25" s="84">
+        <v>50</v>
+      </c>
+      <c r="E25" s="71"/>
+      <c r="F25" s="71"/>
+      <c r="G25" s="71" t="s">
+        <v>49</v>
+      </c>
+      <c r="H25" s="71" t="s">
+        <v>50</v>
+      </c>
+      <c r="I25" s="84" t="s">
+        <v>89</v>
+      </c>
+      <c r="J25" s="71"/>
+      <c r="K25" s="71"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" s="82" t="s">
+        <v>238</v>
+      </c>
+      <c r="B26" s="71" t="s">
+        <v>239</v>
+      </c>
+      <c r="C26" s="82" t="s">
+        <v>63</v>
+      </c>
+      <c r="D26" s="84">
+        <v>50</v>
+      </c>
+      <c r="E26" s="71"/>
+      <c r="F26" s="71"/>
+      <c r="G26" s="71" t="s">
+        <v>49</v>
+      </c>
+      <c r="H26" s="71" t="s">
+        <v>50</v>
+      </c>
+      <c r="I26" s="84" t="s">
+        <v>3</v>
+      </c>
+      <c r="J26" s="71"/>
+      <c r="K26" s="71" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27" s="82" t="s">
+        <v>145</v>
+      </c>
+      <c r="B27" s="71"/>
+      <c r="C27" s="82" t="s">
+        <v>63</v>
+      </c>
+      <c r="D27" s="84">
+        <v>50</v>
+      </c>
+      <c r="E27" s="71"/>
+      <c r="F27" s="71"/>
+      <c r="G27" s="71" t="s">
+        <v>49</v>
+      </c>
+      <c r="H27" s="71" t="s">
+        <v>50</v>
+      </c>
+      <c r="I27" s="84" t="s">
+        <v>91</v>
+      </c>
+      <c r="J27" s="71"/>
+      <c r="K27" s="71" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28" s="82" t="s">
+        <v>143</v>
+      </c>
+      <c r="B28" s="71"/>
+      <c r="C28" s="82" t="s">
+        <v>63</v>
+      </c>
+      <c r="D28" s="84">
+        <v>3</v>
+      </c>
+      <c r="E28" s="71" t="s">
+        <v>93</v>
+      </c>
+      <c r="F28" s="71"/>
+      <c r="G28" s="71" t="s">
+        <v>49</v>
+      </c>
+      <c r="H28" s="71" t="s">
+        <v>50</v>
+      </c>
+      <c r="I28" s="84" t="s">
+        <v>92</v>
+      </c>
+      <c r="J28" s="71"/>
+      <c r="K28" s="71" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A29" s="82" t="s">
+        <v>144</v>
+      </c>
+      <c r="B29" s="71"/>
+      <c r="C29" s="82" t="s">
+        <v>63</v>
+      </c>
+      <c r="D29" s="84">
+        <v>3</v>
+      </c>
+      <c r="E29" s="71" t="s">
+        <v>93</v>
+      </c>
+      <c r="F29" s="71"/>
+      <c r="G29" s="71" t="s">
+        <v>49</v>
+      </c>
+      <c r="H29" s="71" t="s">
+        <v>50</v>
+      </c>
+      <c r="I29" s="84" t="s">
+        <v>96</v>
+      </c>
+      <c r="J29" s="71"/>
+      <c r="K29" s="71" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A30" s="82" t="s">
+        <v>94</v>
+      </c>
+      <c r="B30" s="71"/>
+      <c r="C30" s="82" t="s">
+        <v>63</v>
+      </c>
+      <c r="D30" s="84">
+        <v>3</v>
+      </c>
+      <c r="E30" s="71" t="s">
+        <v>93</v>
+      </c>
+      <c r="F30" s="71"/>
+      <c r="G30" s="71" t="s">
+        <v>49</v>
+      </c>
+      <c r="H30" s="71" t="s">
+        <v>50</v>
+      </c>
+      <c r="I30" s="84" t="s">
+        <v>97</v>
+      </c>
+      <c r="J30" s="71"/>
+      <c r="K30" s="71" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A31" s="82" t="s">
+        <v>95</v>
+      </c>
+      <c r="B31" s="71"/>
+      <c r="C31" s="82" t="s">
+        <v>63</v>
+      </c>
+      <c r="D31" s="84">
+        <v>3</v>
+      </c>
+      <c r="E31" s="71" t="s">
+        <v>93</v>
+      </c>
+      <c r="F31" s="71"/>
+      <c r="G31" s="71" t="s">
+        <v>49</v>
+      </c>
+      <c r="H31" s="71" t="s">
+        <v>50</v>
+      </c>
+      <c r="I31" s="84" t="s">
+        <v>98</v>
+      </c>
+      <c r="J31" s="71"/>
+      <c r="K31" s="71"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A32" s="82" t="s">
+        <v>100</v>
+      </c>
+      <c r="B32" s="71"/>
+      <c r="C32" s="82" t="s">
+        <v>63</v>
+      </c>
+      <c r="D32" s="84">
+        <v>20</v>
+      </c>
+      <c r="E32" s="71"/>
+      <c r="F32" s="71"/>
+      <c r="G32" s="71" t="s">
+        <v>49</v>
+      </c>
+      <c r="H32" s="71" t="s">
+        <v>50</v>
+      </c>
+      <c r="I32" s="84" t="s">
+        <v>101</v>
+      </c>
+      <c r="J32" s="71"/>
+      <c r="K32" s="71"/>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A33" s="82" t="s">
+        <v>102</v>
+      </c>
+      <c r="B33" s="71"/>
+      <c r="C33" s="82" t="s">
+        <v>63</v>
+      </c>
+      <c r="D33" s="84">
+        <v>20</v>
+      </c>
+      <c r="E33" s="71"/>
+      <c r="F33" s="71"/>
+      <c r="G33" s="71" t="s">
+        <v>49</v>
+      </c>
+      <c r="H33" s="71" t="s">
+        <v>50</v>
+      </c>
+      <c r="I33" s="84" t="s">
+        <v>103</v>
+      </c>
+      <c r="J33" s="71"/>
+      <c r="K33" s="71"/>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A34" s="82" t="s">
+        <v>104</v>
+      </c>
+      <c r="B34" s="71"/>
+      <c r="C34" s="82" t="s">
+        <v>63</v>
+      </c>
+      <c r="D34" s="84">
+        <v>50</v>
+      </c>
+      <c r="E34" s="71"/>
+      <c r="F34" s="71"/>
+      <c r="G34" s="71" t="s">
+        <v>49</v>
+      </c>
+      <c r="H34" s="71" t="s">
+        <v>50</v>
+      </c>
+      <c r="I34" s="84" t="s">
+        <v>105</v>
+      </c>
+      <c r="J34" s="71"/>
+      <c r="K34" s="71"/>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A35" s="82" t="s">
+        <v>106</v>
+      </c>
+      <c r="B35" s="71"/>
+      <c r="C35" s="82" t="s">
+        <v>63</v>
+      </c>
+      <c r="D35" s="84">
+        <v>50</v>
+      </c>
+      <c r="E35" s="71"/>
+      <c r="F35" s="71"/>
+      <c r="G35" s="71" t="s">
+        <v>49</v>
+      </c>
+      <c r="H35" s="71" t="s">
+        <v>50</v>
+      </c>
+      <c r="I35" s="84" t="s">
+        <v>107</v>
+      </c>
+      <c r="J35" s="71"/>
+      <c r="K35" s="84"/>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A36" s="82" t="s">
+        <v>146</v>
+      </c>
+      <c r="B36" s="71"/>
+      <c r="C36" s="82" t="s">
+        <v>63</v>
+      </c>
+      <c r="D36" s="71">
+        <v>255</v>
+      </c>
+      <c r="E36" s="71"/>
+      <c r="F36" s="71"/>
+      <c r="G36" s="71" t="s">
+        <v>49</v>
+      </c>
+      <c r="H36" s="71" t="s">
+        <v>50</v>
+      </c>
+      <c r="I36" s="84" t="s">
+        <v>169</v>
+      </c>
+      <c r="J36" s="71"/>
+      <c r="K36" s="84" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A37" s="82" t="s">
+        <v>147</v>
+      </c>
+      <c r="B37" s="71"/>
+      <c r="C37" s="82" t="s">
+        <v>63</v>
+      </c>
+      <c r="D37" s="84">
+        <v>3</v>
+      </c>
+      <c r="E37" s="71" t="s">
+        <v>93</v>
+      </c>
+      <c r="F37" s="71"/>
+      <c r="G37" s="71" t="s">
+        <v>49</v>
+      </c>
+      <c r="H37" s="71" t="s">
+        <v>50</v>
+      </c>
+      <c r="I37" s="71" t="s">
+        <v>148</v>
+      </c>
+      <c r="J37" s="71"/>
+      <c r="K37" s="71" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A38" s="82" t="s">
+        <v>150</v>
+      </c>
+      <c r="B38" s="71"/>
+      <c r="C38" s="82" t="s">
+        <v>63</v>
+      </c>
+      <c r="D38" s="84">
+        <v>3</v>
+      </c>
+      <c r="E38" s="71" t="s">
+        <v>93</v>
+      </c>
+      <c r="F38" s="71"/>
+      <c r="G38" s="71" t="s">
+        <v>49</v>
+      </c>
+      <c r="H38" s="71" t="s">
+        <v>154</v>
+      </c>
+      <c r="I38" s="71" t="s">
+        <v>157</v>
+      </c>
+      <c r="J38" s="71"/>
+      <c r="K38" s="71" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A39" s="82" t="s">
+        <v>151</v>
+      </c>
+      <c r="B39" s="71"/>
+      <c r="C39" s="82" t="s">
+        <v>63</v>
+      </c>
+      <c r="D39" s="84">
+        <v>3</v>
+      </c>
+      <c r="E39" s="71" t="s">
+        <v>93</v>
+      </c>
+      <c r="F39" s="71"/>
+      <c r="G39" s="71" t="s">
+        <v>49</v>
+      </c>
+      <c r="H39" s="71" t="s">
+        <v>50</v>
+      </c>
+      <c r="I39" s="71" t="s">
+        <v>158</v>
+      </c>
+      <c r="J39" s="71"/>
+      <c r="K39" s="71" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A40" s="82" t="s">
+        <v>152</v>
+      </c>
+      <c r="B40" s="71"/>
+      <c r="C40" s="82" t="s">
+        <v>63</v>
+      </c>
+      <c r="D40" s="84">
+        <v>3</v>
+      </c>
+      <c r="E40" s="71" t="s">
+        <v>93</v>
+      </c>
+      <c r="F40" s="71"/>
+      <c r="G40" s="71" t="s">
+        <v>49</v>
+      </c>
+      <c r="H40" s="71" t="s">
+        <v>50</v>
+      </c>
+      <c r="I40" s="71" t="s">
+        <v>153</v>
+      </c>
+      <c r="J40" s="71"/>
+      <c r="K40" s="84"/>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A41" s="82" t="s">
+        <v>163</v>
+      </c>
+      <c r="B41" s="71"/>
+      <c r="C41" s="82" t="s">
+        <v>63</v>
+      </c>
+      <c r="D41" s="84">
+        <v>3</v>
+      </c>
+      <c r="E41" s="71" t="s">
+        <v>93</v>
+      </c>
+      <c r="F41" s="71"/>
+      <c r="G41" s="71" t="s">
+        <v>49</v>
+      </c>
+      <c r="H41" s="84" t="s">
+        <v>159</v>
+      </c>
+      <c r="I41" s="84" t="s">
+        <v>160</v>
+      </c>
+      <c r="J41" s="71"/>
+      <c r="K41" s="71" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A42" s="85" t="s">
+        <v>170</v>
+      </c>
+      <c r="B42" s="86" t="s">
+        <v>171</v>
+      </c>
+      <c r="C42" s="85" t="s">
+        <v>63</v>
+      </c>
+      <c r="D42" s="86">
+        <v>3</v>
+      </c>
+      <c r="E42" s="86" t="s">
+        <v>93</v>
+      </c>
+      <c r="F42" s="86"/>
+      <c r="G42" s="86" t="s">
+        <v>49</v>
+      </c>
+      <c r="H42" s="86" t="s">
+        <v>172</v>
+      </c>
+      <c r="I42" s="86" t="s">
+        <v>173</v>
+      </c>
+      <c r="J42" s="86"/>
+      <c r="K42" s="86" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A43" s="85" t="s">
+        <v>174</v>
+      </c>
+      <c r="B43" s="86" t="s">
+        <v>175</v>
+      </c>
+      <c r="C43" s="85" t="s">
+        <v>63</v>
+      </c>
+      <c r="D43" s="86">
+        <v>3</v>
+      </c>
+      <c r="E43" s="86" t="s">
+        <v>93</v>
+      </c>
+      <c r="F43" s="86"/>
+      <c r="G43" s="86" t="s">
+        <v>49</v>
+      </c>
+      <c r="H43" s="86" t="s">
+        <v>172</v>
+      </c>
+      <c r="I43" s="86" t="s">
+        <v>176</v>
+      </c>
+      <c r="J43" s="86"/>
+      <c r="K43" s="86" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A44" s="85" t="s">
+        <v>177</v>
+      </c>
+      <c r="B44" s="86" t="s">
+        <v>178</v>
+      </c>
+      <c r="C44" s="85" t="s">
+        <v>63</v>
+      </c>
+      <c r="D44" s="86">
+        <v>3</v>
+      </c>
+      <c r="E44" s="86" t="s">
+        <v>93</v>
+      </c>
+      <c r="F44" s="86"/>
+      <c r="G44" s="86" t="s">
+        <v>49</v>
+      </c>
+      <c r="H44" s="86" t="s">
+        <v>172</v>
+      </c>
+      <c r="I44" s="86" t="s">
+        <v>179</v>
+      </c>
+      <c r="J44" s="86"/>
+      <c r="K44" s="86" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A45" s="85" t="s">
+        <v>180</v>
+      </c>
+      <c r="B45" s="86" t="s">
+        <v>181</v>
+      </c>
+      <c r="C45" s="85" t="s">
+        <v>63</v>
+      </c>
+      <c r="D45" s="86">
+        <v>3</v>
+      </c>
+      <c r="E45" s="86" t="s">
+        <v>93</v>
+      </c>
+      <c r="F45" s="86"/>
+      <c r="G45" s="86" t="s">
+        <v>49</v>
+      </c>
+      <c r="H45" s="86" t="s">
+        <v>182</v>
+      </c>
+      <c r="I45" s="86" t="s">
+        <v>183</v>
+      </c>
+      <c r="J45" s="86"/>
+      <c r="K45" s="86" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A46" s="85" t="s">
+        <v>184</v>
+      </c>
+      <c r="B46" s="86" t="s">
+        <v>185</v>
+      </c>
+      <c r="C46" s="85" t="s">
+        <v>63</v>
+      </c>
+      <c r="D46" s="86">
+        <v>3</v>
+      </c>
+      <c r="E46" s="86" t="s">
+        <v>93</v>
+      </c>
+      <c r="F46" s="86"/>
+      <c r="G46" s="86" t="s">
+        <v>49</v>
+      </c>
+      <c r="H46" s="86" t="s">
+        <v>154</v>
+      </c>
+      <c r="I46" s="86" t="s">
+        <v>186</v>
+      </c>
+      <c r="J46" s="86"/>
+      <c r="K46" s="86" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A47" s="85" t="s">
+        <v>187</v>
+      </c>
+      <c r="B47" s="86" t="s">
+        <v>188</v>
+      </c>
+      <c r="C47" s="85" t="s">
+        <v>63</v>
+      </c>
+      <c r="D47" s="86">
+        <v>3</v>
+      </c>
+      <c r="E47" s="86" t="s">
+        <v>93</v>
+      </c>
+      <c r="F47" s="86"/>
+      <c r="G47" s="86" t="s">
+        <v>49</v>
+      </c>
+      <c r="H47" s="86" t="s">
+        <v>154</v>
+      </c>
+      <c r="I47" s="86" t="s">
+        <v>189</v>
+      </c>
+      <c r="J47" s="86"/>
+      <c r="K47" s="86" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A48" s="85" t="s">
+        <v>190</v>
+      </c>
+      <c r="B48" s="86" t="s">
+        <v>191</v>
+      </c>
+      <c r="C48" s="85" t="s">
+        <v>63</v>
+      </c>
+      <c r="D48" s="86">
+        <v>3</v>
+      </c>
+      <c r="E48" s="86" t="s">
+        <v>93</v>
+      </c>
+      <c r="F48" s="86"/>
+      <c r="G48" s="86" t="s">
+        <v>49</v>
+      </c>
+      <c r="H48" s="86" t="s">
+        <v>172</v>
+      </c>
+      <c r="I48" s="86" t="s">
+        <v>192</v>
+      </c>
+      <c r="J48" s="86"/>
+      <c r="K48" s="86" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A49" s="85" t="s">
+        <v>193</v>
+      </c>
+      <c r="B49" s="86" t="s">
+        <v>194</v>
+      </c>
+      <c r="C49" s="85" t="s">
+        <v>63</v>
+      </c>
+      <c r="D49" s="86">
+        <v>3</v>
+      </c>
+      <c r="E49" s="86" t="s">
+        <v>93</v>
+      </c>
+      <c r="F49" s="86"/>
+      <c r="G49" s="86" t="s">
+        <v>49</v>
+      </c>
+      <c r="H49" s="86" t="s">
+        <v>172</v>
+      </c>
+      <c r="I49" s="86" t="s">
+        <v>195</v>
+      </c>
+      <c r="J49" s="86"/>
+      <c r="K49" s="86" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A50" s="85" t="s">
+        <v>196</v>
+      </c>
+      <c r="B50" s="86" t="s">
+        <v>197</v>
+      </c>
+      <c r="C50" s="85" t="s">
+        <v>63</v>
+      </c>
+      <c r="D50" s="86">
+        <v>3</v>
+      </c>
+      <c r="E50" s="86" t="s">
+        <v>93</v>
+      </c>
+      <c r="F50" s="86"/>
+      <c r="G50" s="86" t="s">
+        <v>49</v>
+      </c>
+      <c r="H50" s="86" t="s">
+        <v>172</v>
+      </c>
+      <c r="I50" s="86" t="s">
+        <v>198</v>
+      </c>
+      <c r="J50" s="86"/>
+      <c r="K50" s="86" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A51" s="85" t="s">
+        <v>199</v>
+      </c>
+      <c r="B51" s="86" t="s">
+        <v>200</v>
+      </c>
+      <c r="C51" s="85" t="s">
+        <v>63</v>
+      </c>
+      <c r="D51" s="86">
+        <v>3</v>
+      </c>
+      <c r="E51" s="86" t="s">
+        <v>93</v>
+      </c>
+      <c r="F51" s="86"/>
+      <c r="G51" s="86" t="s">
+        <v>49</v>
+      </c>
+      <c r="H51" s="86" t="s">
+        <v>172</v>
+      </c>
+      <c r="I51" s="86" t="s">
+        <v>201</v>
+      </c>
+      <c r="J51" s="86"/>
+      <c r="K51" s="86" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A52" s="87" t="s">
+        <v>209</v>
+      </c>
+      <c r="B52" s="71" t="s">
+        <v>208</v>
+      </c>
+      <c r="C52" s="87" t="s">
+        <v>63</v>
+      </c>
+      <c r="D52" s="88">
+        <v>3</v>
+      </c>
+      <c r="E52" s="88" t="s">
+        <v>93</v>
+      </c>
+      <c r="F52" s="71"/>
+      <c r="G52" s="88" t="s">
+        <v>49</v>
+      </c>
+      <c r="H52" s="86" t="s">
+        <v>172</v>
+      </c>
+      <c r="I52" s="71" t="s">
+        <v>210</v>
+      </c>
+      <c r="J52" s="71"/>
+      <c r="K52" s="86" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A53" s="71" t="s">
+        <v>256</v>
+      </c>
+      <c r="B53" s="71"/>
+      <c r="C53" s="87" t="s">
+        <v>63</v>
+      </c>
+      <c r="D53" s="88">
+        <v>255</v>
+      </c>
+      <c r="E53" s="71"/>
+      <c r="F53" s="71"/>
+      <c r="G53" s="88" t="s">
+        <v>49</v>
+      </c>
+      <c r="H53" s="71" t="s">
+        <v>50</v>
+      </c>
+      <c r="I53" s="88" t="s">
+        <v>256</v>
+      </c>
+      <c r="J53" s="71"/>
+      <c r="K53" s="71"/>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A54" s="87" t="s">
+        <v>257</v>
+      </c>
+      <c r="B54" s="71"/>
+      <c r="C54" s="87" t="s">
+        <v>63</v>
+      </c>
+      <c r="D54" s="88">
+        <v>100</v>
+      </c>
+      <c r="E54" s="71"/>
+      <c r="F54" s="71"/>
+      <c r="G54" s="88" t="s">
+        <v>49</v>
+      </c>
+      <c r="H54" s="86" t="s">
+        <v>154</v>
+      </c>
+      <c r="I54" s="88" t="s">
+        <v>259</v>
+      </c>
+      <c r="J54" s="71"/>
+      <c r="K54" s="71"/>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A55" s="87" t="s">
+        <v>258</v>
+      </c>
+      <c r="B55" s="71"/>
+      <c r="C55" s="87" t="s">
+        <v>63</v>
+      </c>
+      <c r="D55" s="88">
+        <v>200</v>
+      </c>
+      <c r="E55" s="71"/>
+      <c r="F55" s="71"/>
+      <c r="G55" s="88" t="s">
+        <v>49</v>
+      </c>
+      <c r="H55" s="86" t="s">
+        <v>154</v>
+      </c>
+      <c r="I55" s="88" t="s">
+        <v>260</v>
+      </c>
+      <c r="J55" s="71"/>
+      <c r="K55" s="71"/>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A56" s="87" t="s">
+        <v>261</v>
+      </c>
+      <c r="B56" s="71"/>
+      <c r="C56" s="87" t="s">
+        <v>63</v>
+      </c>
+      <c r="D56" s="88">
+        <v>100</v>
+      </c>
+      <c r="E56" s="71"/>
+      <c r="F56" s="71"/>
+      <c r="G56" s="88" t="s">
+        <v>49</v>
+      </c>
+      <c r="H56" s="71" t="s">
+        <v>50</v>
+      </c>
+      <c r="I56" s="88" t="s">
+        <v>261</v>
+      </c>
+      <c r="J56" s="71"/>
+      <c r="K56" s="71"/>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A57" s="89" t="s">
+        <v>262</v>
+      </c>
+      <c r="C57" s="87" t="s">
+        <v>63</v>
+      </c>
+      <c r="D57" s="88">
+        <v>3</v>
+      </c>
+      <c r="E57" s="88" t="s">
+        <v>93</v>
+      </c>
+      <c r="G57" s="88" t="s">
+        <v>49</v>
+      </c>
+      <c r="H57" s="75" t="s">
+        <v>263</v>
+      </c>
+      <c r="I57" s="90" t="s">
+        <v>262</v>
+      </c>
+      <c r="K57" s="91" t="s">
+        <v>264</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="44" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
@@ -4957,7 +6751,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K17"/>
   <sheetViews>
@@ -5287,7 +7081,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K14"/>
   <sheetViews>
@@ -5595,7 +7389,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K10"/>
   <sheetViews>
@@ -5779,7 +7573,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K10"/>
   <sheetViews>
@@ -5905,263 +7699,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K10"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16" style="27" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="44.42578125" style="27" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.28515625" style="27" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4.5703125" style="27" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.140625" style="27" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" style="27"/>
-    <col min="7" max="7" width="14" style="27" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.28515625" style="27" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.85546875" style="27" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.5703125" style="27" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="68.28515625" style="27" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:11" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="29" t="s">
-        <v>17</v>
-      </c>
-      <c r="B1" s="28" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="30" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="30" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="30" t="s">
-        <v>20</v>
-      </c>
-      <c r="B4" s="27" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="B5" s="27" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="30" t="s">
-        <v>22</v>
-      </c>
-      <c r="B6" s="27" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="33" t="s">
-        <v>25</v>
-      </c>
-      <c r="B8" s="33" t="s">
-        <v>20</v>
-      </c>
-      <c r="C8" s="33" t="s">
-        <v>26</v>
-      </c>
-      <c r="D8" s="33" t="s">
-        <v>22</v>
-      </c>
-      <c r="E8" s="34" t="s">
-        <v>27</v>
-      </c>
-      <c r="F8" s="33" t="s">
-        <v>29</v>
-      </c>
-      <c r="G8" s="33" t="s">
-        <v>30</v>
-      </c>
-      <c r="H8" s="33" t="s">
-        <v>31</v>
-      </c>
-      <c r="I8" s="33" t="s">
-        <v>32</v>
-      </c>
-      <c r="J8" s="33" t="s">
-        <v>33</v>
-      </c>
-      <c r="K8" s="33" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="31"/>
-      <c r="B9" s="32"/>
-      <c r="C9" s="32"/>
-      <c r="D9" s="32"/>
-      <c r="E9" s="32"/>
-      <c r="F9" s="32"/>
-      <c r="G9" s="32"/>
-      <c r="H9" s="32"/>
-      <c r="I9" s="32"/>
-      <c r="J9" s="32"/>
-      <c r="K9" s="32"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="32"/>
-      <c r="B10" s="32"/>
-      <c r="C10" s="32"/>
-      <c r="D10" s="32"/>
-      <c r="E10" s="32"/>
-      <c r="F10" s="32"/>
-      <c r="G10" s="32"/>
-      <c r="H10" s="35"/>
-      <c r="I10" s="32"/>
-      <c r="J10" s="32"/>
-      <c r="K10" s="32"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K10"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16" style="27" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="44.42578125" style="27" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.28515625" style="27" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4.5703125" style="27" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.140625" style="27" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" style="27"/>
-    <col min="7" max="7" width="14" style="27" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.28515625" style="27" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.85546875" style="27" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.5703125" style="27" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="68.28515625" style="27" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:11" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="29" t="s">
-        <v>17</v>
-      </c>
-      <c r="B1" s="28" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="30" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="30" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="30" t="s">
-        <v>20</v>
-      </c>
-      <c r="B4" s="27" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="B5" s="27" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="30" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="33" t="s">
-        <v>25</v>
-      </c>
-      <c r="B8" s="33" t="s">
-        <v>20</v>
-      </c>
-      <c r="C8" s="33" t="s">
-        <v>26</v>
-      </c>
-      <c r="D8" s="33" t="s">
-        <v>22</v>
-      </c>
-      <c r="E8" s="34" t="s">
-        <v>27</v>
-      </c>
-      <c r="F8" s="33" t="s">
-        <v>29</v>
-      </c>
-      <c r="G8" s="33" t="s">
-        <v>30</v>
-      </c>
-      <c r="H8" s="33" t="s">
-        <v>31</v>
-      </c>
-      <c r="I8" s="33" t="s">
-        <v>32</v>
-      </c>
-      <c r="J8" s="33" t="s">
-        <v>33</v>
-      </c>
-      <c r="K8" s="33" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="31"/>
-      <c r="B9" s="32"/>
-      <c r="C9" s="32"/>
-      <c r="D9" s="32"/>
-      <c r="E9" s="32"/>
-      <c r="F9" s="32"/>
-      <c r="G9" s="32"/>
-      <c r="H9" s="32"/>
-      <c r="I9" s="32"/>
-      <c r="J9" s="32"/>
-      <c r="K9" s="32"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="32"/>
-      <c r="B10" s="32"/>
-      <c r="C10" s="32"/>
-      <c r="D10" s="32"/>
-      <c r="E10" s="32"/>
-      <c r="F10" s="32"/>
-      <c r="G10" s="32"/>
-      <c r="H10" s="35"/>
-      <c r="I10" s="32"/>
-      <c r="J10" s="32"/>
-      <c r="K10" s="32"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
update bus matrix for riskman to add tables for feedback module.
</commit_message>
<xml_diff>
--- a/Matrix_Bus/RiskMan Bus Matrix.xlsx
+++ b/Matrix_Bus/RiskMan Bus Matrix.xlsx
@@ -4,32 +4,33 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="7050" windowWidth="24090" windowHeight="3075" firstSheet="8" activeTab="15"/>
+    <workbookView xWindow="-90" yWindow="7050" windowWidth="24090" windowHeight="3075" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Bus Matrix" sheetId="1" r:id="rId1"/>
     <sheet name="incident_fact" sheetId="2" r:id="rId2"/>
     <sheet name="feedback_fact" sheetId="19" r:id="rId3"/>
-    <sheet name="Sheet2" sheetId="20" r:id="rId4"/>
-    <sheet name="ContributingFactors_fact" sheetId="18" r:id="rId5"/>
-    <sheet name="incident_history_fact" sheetId="17" r:id="rId6"/>
-    <sheet name="person_dim" sheetId="6" r:id="rId7"/>
-    <sheet name="Employee_DIM" sheetId="5" r:id="rId8"/>
-    <sheet name="Date_DIM" sheetId="7" r:id="rId9"/>
-    <sheet name="Portfolio_DIM" sheetId="9" r:id="rId10"/>
-    <sheet name="Service_Stream_DIM" sheetId="10" r:id="rId11"/>
-    <sheet name="Program_DIM" sheetId="11" r:id="rId12"/>
-    <sheet name="Incident_Type_DIM" sheetId="13" r:id="rId13"/>
-    <sheet name="action_dim" sheetId="15" r:id="rId14"/>
-    <sheet name="incident_type_fact" sheetId="14" r:id="rId15"/>
-    <sheet name="incident_action_fact" sheetId="16" r:id="rId16"/>
+    <sheet name="feedbak_bridge" sheetId="21" r:id="rId4"/>
+    <sheet name="feedback_details_fact" sheetId="20" r:id="rId5"/>
+    <sheet name="ContributingFactors_fact" sheetId="18" r:id="rId6"/>
+    <sheet name="incident_history_fact" sheetId="17" r:id="rId7"/>
+    <sheet name="person_dim" sheetId="6" r:id="rId8"/>
+    <sheet name="Employee_DIM" sheetId="5" r:id="rId9"/>
+    <sheet name="Date_DIM" sheetId="7" r:id="rId10"/>
+    <sheet name="Portfolio_DIM" sheetId="9" r:id="rId11"/>
+    <sheet name="Service_Stream_DIM" sheetId="10" r:id="rId12"/>
+    <sheet name="Program_DIM" sheetId="11" r:id="rId13"/>
+    <sheet name="Incident_Type_DIM" sheetId="13" r:id="rId14"/>
+    <sheet name="action_dim" sheetId="15" r:id="rId15"/>
+    <sheet name="incident_type_fact" sheetId="14" r:id="rId16"/>
+    <sheet name="incident_action_fact" sheetId="16" r:id="rId17"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1155" uniqueCount="281">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1233" uniqueCount="298">
   <si>
     <t>Category</t>
   </si>
@@ -906,6 +907,60 @@
   </si>
   <si>
     <t>feedback_key</t>
+  </si>
+  <si>
+    <t>Feedbak_Details_Fact</t>
+  </si>
+  <si>
+    <t>Feedback_Details_Fact</t>
+  </si>
+  <si>
+    <t>Used to store feedback details</t>
+  </si>
+  <si>
+    <t>fd_key</t>
+  </si>
+  <si>
+    <t>batchid</t>
+  </si>
+  <si>
+    <t>fieldname</t>
+  </si>
+  <si>
+    <t>valuestring</t>
+  </si>
+  <si>
+    <t>nvarchar</t>
+  </si>
+  <si>
+    <t>max</t>
+  </si>
+  <si>
+    <t>frm_data</t>
+  </si>
+  <si>
+    <t>Feedbak_Bridge</t>
+  </si>
+  <si>
+    <t>Feedback_Bridge</t>
+  </si>
+  <si>
+    <t>Used to store ids to link feeback_fact and feedback_details_fact</t>
+  </si>
+  <si>
+    <t>fb_key</t>
+  </si>
+  <si>
+    <t>feedback_fact</t>
+  </si>
+  <si>
+    <t>feedback_details_fact</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   select t1.fbissue_id,t1.fbissueprevrecid,t3.BatchID 
+   from extract_riskman.FBIssue_IFR as t1
+   inner join extract_riskman.frm_record as t2 on t1.fbissueprevrecid= t2.KeyData
+   inner join  extract_riskman.FRM_BATCH as t3 on t2.RecordID=t3.RecordID</t>
   </si>
 </sst>
 </file>
@@ -995,7 +1050,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="26">
+  <borders count="28">
     <border>
       <left/>
       <right/>
@@ -1318,11 +1373,37 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="92">
+  <cellXfs count="98">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -1504,6 +1585,18 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2096,6 +2189,134 @@
   <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16" style="27" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="44.42578125" style="27" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.28515625" style="27" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.5703125" style="27" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.140625" style="27" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" style="27"/>
+    <col min="7" max="7" width="14" style="27" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.28515625" style="27" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.85546875" style="27" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.5703125" style="27" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="68.28515625" style="27" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A1" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="28" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="30" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="30" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="30" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="27" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="30" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="27" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="33" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" s="33" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="33" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" s="33" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8" s="34" t="s">
+        <v>27</v>
+      </c>
+      <c r="F8" s="33" t="s">
+        <v>29</v>
+      </c>
+      <c r="G8" s="33" t="s">
+        <v>30</v>
+      </c>
+      <c r="H8" s="33" t="s">
+        <v>31</v>
+      </c>
+      <c r="I8" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="J8" s="33" t="s">
+        <v>33</v>
+      </c>
+      <c r="K8" s="33" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="31"/>
+      <c r="B9" s="32"/>
+      <c r="C9" s="32"/>
+      <c r="D9" s="32"/>
+      <c r="E9" s="32"/>
+      <c r="F9" s="32"/>
+      <c r="G9" s="32"/>
+      <c r="H9" s="32"/>
+      <c r="I9" s="32"/>
+      <c r="J9" s="32"/>
+      <c r="K9" s="32"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="32"/>
+      <c r="B10" s="32"/>
+      <c r="C10" s="32"/>
+      <c r="D10" s="32"/>
+      <c r="E10" s="32"/>
+      <c r="F10" s="32"/>
+      <c r="G10" s="32"/>
+      <c r="H10" s="35"/>
+      <c r="I10" s="32"/>
+      <c r="J10" s="32"/>
+      <c r="K10" s="32"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
       <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
@@ -2154,134 +2375,6 @@
       </c>
       <c r="B6" s="27" t="s">
         <v>117</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="33" t="s">
-        <v>25</v>
-      </c>
-      <c r="B8" s="33" t="s">
-        <v>20</v>
-      </c>
-      <c r="C8" s="33" t="s">
-        <v>26</v>
-      </c>
-      <c r="D8" s="33" t="s">
-        <v>22</v>
-      </c>
-      <c r="E8" s="34" t="s">
-        <v>27</v>
-      </c>
-      <c r="F8" s="33" t="s">
-        <v>29</v>
-      </c>
-      <c r="G8" s="33" t="s">
-        <v>30</v>
-      </c>
-      <c r="H8" s="33" t="s">
-        <v>31</v>
-      </c>
-      <c r="I8" s="33" t="s">
-        <v>32</v>
-      </c>
-      <c r="J8" s="33" t="s">
-        <v>33</v>
-      </c>
-      <c r="K8" s="33" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="31"/>
-      <c r="B9" s="32"/>
-      <c r="C9" s="32"/>
-      <c r="D9" s="32"/>
-      <c r="E9" s="32"/>
-      <c r="F9" s="32"/>
-      <c r="G9" s="32"/>
-      <c r="H9" s="32"/>
-      <c r="I9" s="32"/>
-      <c r="J9" s="32"/>
-      <c r="K9" s="32"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="32"/>
-      <c r="B10" s="32"/>
-      <c r="C10" s="32"/>
-      <c r="D10" s="32"/>
-      <c r="E10" s="32"/>
-      <c r="F10" s="32"/>
-      <c r="G10" s="32"/>
-      <c r="H10" s="35"/>
-      <c r="I10" s="32"/>
-      <c r="J10" s="32"/>
-      <c r="K10" s="32"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K10"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16" style="27" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="44.42578125" style="27" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.28515625" style="27" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4.5703125" style="27" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.140625" style="27" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" style="27"/>
-    <col min="7" max="7" width="14" style="27" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.28515625" style="27" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.85546875" style="27" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.5703125" style="27" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="68.28515625" style="27" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:11" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="29" t="s">
-        <v>17</v>
-      </c>
-      <c r="B1" s="28" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="30" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="30" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="30" t="s">
-        <v>20</v>
-      </c>
-      <c r="B4" s="27" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="B5" s="27" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="30" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -2378,7 +2471,7 @@
         <v>17</v>
       </c>
       <c r="B1" s="28" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -2479,6 +2572,134 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16" style="27" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="44.42578125" style="27" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.28515625" style="27" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.5703125" style="27" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.140625" style="27" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" style="27"/>
+    <col min="7" max="7" width="14" style="27" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.28515625" style="27" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.85546875" style="27" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.5703125" style="27" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="68.28515625" style="27" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A1" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="28" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="30" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="30" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="30" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="27" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="27" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="30" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="33" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" s="33" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="33" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" s="33" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8" s="34" t="s">
+        <v>27</v>
+      </c>
+      <c r="F8" s="33" t="s">
+        <v>29</v>
+      </c>
+      <c r="G8" s="33" t="s">
+        <v>30</v>
+      </c>
+      <c r="H8" s="33" t="s">
+        <v>31</v>
+      </c>
+      <c r="I8" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="J8" s="33" t="s">
+        <v>33</v>
+      </c>
+      <c r="K8" s="33" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="31"/>
+      <c r="B9" s="32"/>
+      <c r="C9" s="32"/>
+      <c r="D9" s="32"/>
+      <c r="E9" s="32"/>
+      <c r="F9" s="32"/>
+      <c r="G9" s="32"/>
+      <c r="H9" s="32"/>
+      <c r="I9" s="32"/>
+      <c r="J9" s="32"/>
+      <c r="K9" s="32"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="32"/>
+      <c r="B10" s="32"/>
+      <c r="C10" s="32"/>
+      <c r="D10" s="32"/>
+      <c r="E10" s="32"/>
+      <c r="F10" s="32"/>
+      <c r="G10" s="32"/>
+      <c r="H10" s="35"/>
+      <c r="I10" s="32"/>
+      <c r="J10" s="32"/>
+      <c r="K10" s="32"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K12"/>
   <sheetViews>
@@ -2689,7 +2910,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K19"/>
   <sheetViews>
@@ -3092,7 +3313,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K12"/>
   <sheetViews>
@@ -3355,11 +3576,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -5075,8 +5296,8 @@
   </sheetPr>
   <dimension ref="A1:L57"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6518,22 +6739,527 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <sheetPr>
+    <tabColor rgb="FFFFFF00"/>
+  </sheetPr>
+  <dimension ref="A1:K11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="23.7109375" customWidth="1"/>
+    <col min="2" max="2" width="32.5703125" customWidth="1"/>
+    <col min="8" max="8" width="25" customWidth="1"/>
+    <col min="9" max="9" width="29.42578125" customWidth="1"/>
+    <col min="10" max="10" width="12.85546875" customWidth="1"/>
+    <col min="11" max="11" width="40" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A1" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="28" t="s">
+        <v>291</v>
+      </c>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="27"/>
+      <c r="I1" s="27"/>
+      <c r="J1" s="27"/>
+      <c r="K1" s="27"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="30" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27"/>
+      <c r="H2" s="27"/>
+      <c r="I2" s="27"/>
+      <c r="J2" s="27"/>
+      <c r="K2" s="27"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="27" t="s">
+        <v>292</v>
+      </c>
+      <c r="C3" s="27"/>
+      <c r="D3" s="27"/>
+      <c r="E3" s="27"/>
+      <c r="F3" s="27"/>
+      <c r="G3" s="27"/>
+      <c r="H3" s="27"/>
+      <c r="I3" s="27"/>
+      <c r="J3" s="27"/>
+      <c r="K3" s="27"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="30" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="27" t="s">
+        <v>293</v>
+      </c>
+      <c r="C4" s="27"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
+      <c r="F4" s="27"/>
+      <c r="G4" s="27"/>
+      <c r="H4" s="27"/>
+      <c r="I4" s="27"/>
+      <c r="J4" s="27"/>
+      <c r="K4" s="27"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="27" t="s">
+        <v>76</v>
+      </c>
+      <c r="C5" s="27"/>
+      <c r="D5" s="27"/>
+      <c r="E5" s="27"/>
+      <c r="F5" s="27"/>
+      <c r="G5" s="27"/>
+      <c r="H5" s="27"/>
+      <c r="I5" s="27"/>
+      <c r="J5" s="27"/>
+      <c r="K5" s="27"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="27" t="s">
+        <v>133</v>
+      </c>
+      <c r="C6" s="27"/>
+      <c r="D6" s="27"/>
+      <c r="E6" s="27"/>
+      <c r="F6" s="27"/>
+      <c r="G6" s="27"/>
+      <c r="H6" s="27"/>
+      <c r="I6" s="27"/>
+      <c r="J6" s="27"/>
+      <c r="K6" s="27"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="27"/>
+      <c r="B7" s="27"/>
+      <c r="C7" s="27"/>
+      <c r="D7" s="27"/>
+      <c r="E7" s="27"/>
+      <c r="F7" s="27"/>
+      <c r="G7" s="27"/>
+      <c r="H7" s="27"/>
+      <c r="I7" s="27"/>
+      <c r="J7" s="27"/>
+      <c r="K7" s="27"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="F8" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="G8" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="H8" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="I8" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="J8" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="K8" s="13" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="94" t="s">
+        <v>294</v>
+      </c>
+      <c r="B9" s="95"/>
+      <c r="C9" s="95" t="s">
+        <v>62</v>
+      </c>
+      <c r="D9" s="95"/>
+      <c r="E9" s="95"/>
+      <c r="F9" s="95"/>
+      <c r="G9" s="95"/>
+      <c r="H9" s="95"/>
+      <c r="I9" s="95"/>
+      <c r="J9" s="95"/>
+      <c r="K9" s="95"/>
+    </row>
+    <row r="10" spans="1:11" ht="120" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="95" t="s">
+        <v>135</v>
+      </c>
+      <c r="B10" s="95"/>
+      <c r="C10" s="95" t="s">
+        <v>62</v>
+      </c>
+      <c r="D10" s="95"/>
+      <c r="E10" s="95"/>
+      <c r="F10" s="95"/>
+      <c r="G10" s="95"/>
+      <c r="H10" s="95" t="s">
+        <v>295</v>
+      </c>
+      <c r="I10" s="95" t="s">
+        <v>135</v>
+      </c>
+      <c r="J10" s="95"/>
+      <c r="K10" s="96" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="95" t="s">
+        <v>285</v>
+      </c>
+      <c r="B11" s="95"/>
+      <c r="C11" s="95" t="s">
+        <v>62</v>
+      </c>
+      <c r="D11" s="95"/>
+      <c r="E11" s="95"/>
+      <c r="F11" s="95"/>
+      <c r="G11" s="95"/>
+      <c r="H11" s="95" t="s">
+        <v>296</v>
+      </c>
+      <c r="I11" s="95" t="s">
+        <v>285</v>
+      </c>
+      <c r="J11" s="95"/>
+      <c r="K11" s="97"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="K10:K11"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FFFFFF00"/>
+  </sheetPr>
+  <dimension ref="A1:K13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="27.5703125" customWidth="1"/>
+    <col min="2" max="2" width="47.7109375" customWidth="1"/>
+    <col min="3" max="3" width="11.85546875" customWidth="1"/>
+    <col min="7" max="7" width="16.140625" customWidth="1"/>
+    <col min="8" max="8" width="23" customWidth="1"/>
+    <col min="9" max="9" width="23.140625" customWidth="1"/>
+    <col min="10" max="10" width="19.5703125" customWidth="1"/>
+    <col min="11" max="11" width="18.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A1" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="28" t="s">
+        <v>281</v>
+      </c>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="27"/>
+      <c r="I1" s="27"/>
+      <c r="J1" s="27"/>
+      <c r="K1" s="27"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="30" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27"/>
+      <c r="H2" s="27"/>
+      <c r="I2" s="27"/>
+      <c r="J2" s="27"/>
+      <c r="K2" s="27"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="27" t="s">
+        <v>282</v>
+      </c>
+      <c r="C3" s="27"/>
+      <c r="D3" s="27"/>
+      <c r="E3" s="27"/>
+      <c r="F3" s="27"/>
+      <c r="G3" s="27"/>
+      <c r="H3" s="27"/>
+      <c r="I3" s="27"/>
+      <c r="J3" s="27"/>
+      <c r="K3" s="27"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="30" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="27" t="s">
+        <v>283</v>
+      </c>
+      <c r="C4" s="27"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
+      <c r="F4" s="27"/>
+      <c r="G4" s="27"/>
+      <c r="H4" s="27"/>
+      <c r="I4" s="27"/>
+      <c r="J4" s="27"/>
+      <c r="K4" s="27"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="27" t="s">
+        <v>76</v>
+      </c>
+      <c r="C5" s="27"/>
+      <c r="D5" s="27"/>
+      <c r="E5" s="27"/>
+      <c r="F5" s="27"/>
+      <c r="G5" s="27"/>
+      <c r="H5" s="27"/>
+      <c r="I5" s="27"/>
+      <c r="J5" s="27"/>
+      <c r="K5" s="27"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="27" t="s">
+        <v>133</v>
+      </c>
+      <c r="C6" s="27"/>
+      <c r="D6" s="27"/>
+      <c r="E6" s="27"/>
+      <c r="F6" s="27"/>
+      <c r="G6" s="27"/>
+      <c r="H6" s="27"/>
+      <c r="I6" s="27"/>
+      <c r="J6" s="27"/>
+      <c r="K6" s="27"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="27"/>
+      <c r="B7" s="27"/>
+      <c r="C7" s="27"/>
+      <c r="D7" s="27"/>
+      <c r="E7" s="27"/>
+      <c r="F7" s="27"/>
+      <c r="G7" s="27"/>
+      <c r="H7" s="27"/>
+      <c r="I7" s="27"/>
+      <c r="J7" s="27"/>
+      <c r="K7" s="27"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="F8" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="G8" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="H8" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="I8" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="J8" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="K8" s="13" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="93" t="s">
+        <v>284</v>
+      </c>
+      <c r="B9" s="71"/>
+      <c r="C9" s="71" t="s">
+        <v>62</v>
+      </c>
+      <c r="D9" s="71"/>
+      <c r="E9" s="71"/>
+      <c r="F9" s="71"/>
+      <c r="G9" s="71"/>
+      <c r="H9" s="71"/>
+      <c r="I9" s="71"/>
+      <c r="J9" s="71"/>
+      <c r="K9" s="71"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="93" t="s">
+        <v>285</v>
+      </c>
+      <c r="B10" s="71"/>
+      <c r="C10" s="71" t="s">
+        <v>62</v>
+      </c>
+      <c r="D10" s="71"/>
+      <c r="E10" s="71"/>
+      <c r="F10" s="71"/>
+      <c r="G10" s="71" t="s">
+        <v>49</v>
+      </c>
+      <c r="H10" s="71" t="s">
+        <v>290</v>
+      </c>
+      <c r="I10" s="93" t="s">
+        <v>285</v>
+      </c>
+      <c r="J10" s="71" t="s">
+        <v>62</v>
+      </c>
+      <c r="K10" s="71"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="93" t="s">
+        <v>286</v>
+      </c>
+      <c r="B11" s="71"/>
+      <c r="C11" s="71" t="s">
+        <v>63</v>
+      </c>
+      <c r="D11" s="71">
+        <v>50</v>
+      </c>
+      <c r="E11" s="71"/>
+      <c r="F11" s="71"/>
+      <c r="G11" s="71" t="s">
+        <v>49</v>
+      </c>
+      <c r="H11" s="71" t="s">
+        <v>290</v>
+      </c>
+      <c r="I11" s="93" t="s">
+        <v>286</v>
+      </c>
+      <c r="J11" s="71" t="s">
+        <v>63</v>
+      </c>
+      <c r="K11" s="71"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="93" t="s">
+        <v>287</v>
+      </c>
+      <c r="B12" s="71"/>
+      <c r="C12" s="71" t="s">
+        <v>288</v>
+      </c>
+      <c r="D12" s="71" t="s">
+        <v>289</v>
+      </c>
+      <c r="E12" s="71"/>
+      <c r="F12" s="71"/>
+      <c r="G12" s="71" t="s">
+        <v>49</v>
+      </c>
+      <c r="H12" s="71" t="s">
+        <v>290</v>
+      </c>
+      <c r="I12" s="93" t="s">
+        <v>287</v>
+      </c>
+      <c r="J12" s="71" t="s">
+        <v>288</v>
+      </c>
+      <c r="K12" s="71"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="92"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M10" sqref="M10"/>
+      <selection sqref="A1:K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6751,7 +7477,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K17"/>
   <sheetViews>
@@ -7081,7 +7807,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K14"/>
   <sheetViews>
@@ -7389,7 +8115,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K10"/>
   <sheetViews>
@@ -7571,132 +8297,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K10"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16" style="27" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="44.42578125" style="27" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.28515625" style="27" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4.5703125" style="27" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.140625" style="27" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" style="27"/>
-    <col min="7" max="7" width="14" style="27" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.28515625" style="27" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.85546875" style="27" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.5703125" style="27" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="68.28515625" style="27" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:11" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="29" t="s">
-        <v>17</v>
-      </c>
-      <c r="B1" s="28" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="30" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="30" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="30" t="s">
-        <v>20</v>
-      </c>
-      <c r="B4" s="27" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="30" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="30" t="s">
-        <v>22</v>
-      </c>
-      <c r="B6" s="27" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="33" t="s">
-        <v>25</v>
-      </c>
-      <c r="B8" s="33" t="s">
-        <v>20</v>
-      </c>
-      <c r="C8" s="33" t="s">
-        <v>26</v>
-      </c>
-      <c r="D8" s="33" t="s">
-        <v>22</v>
-      </c>
-      <c r="E8" s="34" t="s">
-        <v>27</v>
-      </c>
-      <c r="F8" s="33" t="s">
-        <v>29</v>
-      </c>
-      <c r="G8" s="33" t="s">
-        <v>30</v>
-      </c>
-      <c r="H8" s="33" t="s">
-        <v>31</v>
-      </c>
-      <c r="I8" s="33" t="s">
-        <v>32</v>
-      </c>
-      <c r="J8" s="33" t="s">
-        <v>33</v>
-      </c>
-      <c r="K8" s="33" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="31"/>
-      <c r="B9" s="32"/>
-      <c r="C9" s="32"/>
-      <c r="D9" s="32"/>
-      <c r="E9" s="32"/>
-      <c r="F9" s="32"/>
-      <c r="G9" s="32"/>
-      <c r="H9" s="32"/>
-      <c r="I9" s="32"/>
-      <c r="J9" s="32"/>
-      <c r="K9" s="32"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="32"/>
-      <c r="B10" s="32"/>
-      <c r="C10" s="32"/>
-      <c r="D10" s="32"/>
-      <c r="E10" s="32"/>
-      <c r="F10" s="32"/>
-      <c r="G10" s="32"/>
-      <c r="H10" s="35"/>
-      <c r="I10" s="32"/>
-      <c r="J10" s="32"/>
-      <c r="K10" s="32"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
update etl and matrix bus for feedbak module in riskman data mart.
</commit_message>
<xml_diff>
--- a/Matrix_Bus/RiskMan Bus Matrix.xlsx
+++ b/Matrix_Bus/RiskMan Bus Matrix.xlsx
@@ -10,8 +10,8 @@
     <sheet name="Bus Matrix" sheetId="1" r:id="rId1"/>
     <sheet name="incident_fact" sheetId="2" r:id="rId2"/>
     <sheet name="feedback_fact" sheetId="19" r:id="rId3"/>
-    <sheet name="feedbak_bridge" sheetId="21" r:id="rId4"/>
-    <sheet name="feedback_details_fact" sheetId="20" r:id="rId5"/>
+    <sheet name="feedbak_issue_bridge" sheetId="21" r:id="rId4"/>
+    <sheet name="feedback_issue_fact" sheetId="20" r:id="rId5"/>
     <sheet name="ContributingFactors_fact" sheetId="18" r:id="rId6"/>
     <sheet name="incident_history_fact" sheetId="17" r:id="rId7"/>
     <sheet name="person_dim" sheetId="6" r:id="rId8"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1233" uniqueCount="298">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1163" uniqueCount="355">
   <si>
     <t>Category</t>
   </si>
@@ -900,24 +900,12 @@
     <t>Feedback Fact</t>
   </si>
   <si>
-    <t>Used to store feedbacks for incidents</t>
-  </si>
-  <si>
     <t>SubModule='RMFeedback'</t>
   </si>
   <si>
     <t>feedback_key</t>
   </si>
   <si>
-    <t>Feedbak_Details_Fact</t>
-  </si>
-  <si>
-    <t>Feedback_Details_Fact</t>
-  </si>
-  <si>
-    <t>Used to store feedback details</t>
-  </si>
-  <si>
     <t>fd_key</t>
   </si>
   <si>
@@ -937,15 +925,6 @@
   </si>
   <si>
     <t>frm_data</t>
-  </si>
-  <si>
-    <t>Feedbak_Bridge</t>
-  </si>
-  <si>
-    <t>Feedback_Bridge</t>
-  </si>
-  <si>
-    <t>Used to store ids to link feeback_fact and feedback_details_fact</t>
   </si>
   <si>
     <t>fb_key</t>
@@ -961,13 +940,205 @@
    from extract_riskman.FBIssue_IFR as t1
    inner join extract_riskman.frm_record as t2 on t1.fbissueprevrecid= t2.KeyData
    inner join  extract_riskman.FRM_BATCH as t3 on t2.RecordID=t3.RecordID</t>
+  </si>
+  <si>
+    <t>[ID]</t>
+  </si>
+  <si>
+    <t>[DisplayID]</t>
+  </si>
+  <si>
+    <t>IncidentInvolved</t>
+  </si>
+  <si>
+    <t>[FBModeRecieved]</t>
+  </si>
+  <si>
+    <t>[FBRelateClient]</t>
+  </si>
+  <si>
+    <t>[FBRelateStaff]</t>
+  </si>
+  <si>
+    <t>FBAssocInc</t>
+  </si>
+  <si>
+    <t>AdditionalRef</t>
+  </si>
+  <si>
+    <t>[Site]</t>
+  </si>
+  <si>
+    <t>[Incident_Location]</t>
+  </si>
+  <si>
+    <t>FBCompStatus</t>
+  </si>
+  <si>
+    <t>FBCompStatusOther</t>
+  </si>
+  <si>
+    <t>[FBCompAnon]</t>
+  </si>
+  <si>
+    <t>[FBCompRelationship]</t>
+  </si>
+  <si>
+    <t>[FBAckDate]</t>
+  </si>
+  <si>
+    <t>FBFirstFormalDate</t>
+  </si>
+  <si>
+    <t>[Outcome]</t>
+  </si>
+  <si>
+    <t>InvestigationFinding</t>
+  </si>
+  <si>
+    <t>FBObjectives</t>
+  </si>
+  <si>
+    <t>FBExtAgency</t>
+  </si>
+  <si>
+    <t>FBExtAgencyName</t>
+  </si>
+  <si>
+    <t>FBIsClosed</t>
+  </si>
+  <si>
+    <t>[Comment]</t>
+  </si>
+  <si>
+    <t>FBOutcome</t>
+  </si>
+  <si>
+    <t>Record ID (KEY)</t>
+  </si>
+  <si>
+    <t>Feedback ID</t>
+  </si>
+  <si>
+    <t>Source of Notification</t>
+  </si>
+  <si>
+    <t>Does this feedback relate to a Customer?</t>
+  </si>
+  <si>
+    <t>Does this feedback relate to staff?</t>
+  </si>
+  <si>
+    <t>Related to Incident</t>
+  </si>
+  <si>
+    <t>Incident Sources</t>
+  </si>
+  <si>
+    <t>Service</t>
+  </si>
+  <si>
+    <t>Who is providing feedback?</t>
+  </si>
+  <si>
+    <t>Who is Providing Feedback? Other</t>
+  </si>
+  <si>
+    <t>Anonymous (Person Lodging)</t>
+  </si>
+  <si>
+    <t>Relationship to Customer</t>
+  </si>
+  <si>
+    <t>Date acknowledged?</t>
+  </si>
+  <si>
+    <t>Response Date?</t>
+  </si>
+  <si>
+    <t>Feedback Severity Rating</t>
+  </si>
+  <si>
+    <t>Issue Group</t>
+  </si>
+  <si>
+    <t>Issue Category</t>
+  </si>
+  <si>
+    <t>Investigation Notes</t>
+  </si>
+  <si>
+    <t>Objectives</t>
+  </si>
+  <si>
+    <t>Has the complainant raised this complaint with an external agency?</t>
+  </si>
+  <si>
+    <t>External Agency Name</t>
+  </si>
+  <si>
+    <t>Is this complaint closed?</t>
+  </si>
+  <si>
+    <t>Outcome Details</t>
+  </si>
+  <si>
+    <t>[FBDetail_IFR]</t>
+  </si>
+  <si>
+    <t>[FBDetail_IFR][FBDetail_ID] Join to [IncidentsForReview][ID]</t>
+  </si>
+  <si>
+    <t>[IncidentsForReview]</t>
+  </si>
+  <si>
+    <t>[FBComplainant_IFR]</t>
+  </si>
+  <si>
+    <t>[FBComplainant_IFR][FBComplainant_ID] Join to [IncidentsForReview][ID]</t>
+  </si>
+  <si>
+    <t>[FBInvestigation_IFR]</t>
+  </si>
+  <si>
+    <t>[FBDetail1_IFR]</t>
+  </si>
+  <si>
+    <t>Should Join to Incident_For_Review on FBInvestigation_ID to ID - Could be many to one relationship</t>
+  </si>
+  <si>
+    <t>[FBDetail1_IFR][FBDetail1_ID] Join to [IncidentsForReview][ID]</t>
+  </si>
+  <si>
+    <t>Could be multiple for each incident</t>
+  </si>
+  <si>
+    <t>Base_id</t>
+  </si>
+  <si>
+    <t>Link to feeback_issue_bridge and feeback_issue_fact</t>
+  </si>
+  <si>
+    <t>Used to store feedbacks information</t>
+  </si>
+  <si>
+    <t>Feedbak_Issue_Bridge</t>
+  </si>
+  <si>
+    <t>Feedbak_Issue_Fact</t>
+  </si>
+  <si>
+    <t>Used to store feedback issue details</t>
+  </si>
+  <si>
+    <t>Used to store ids to link feeback_fact and feedback_issue_fact</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1029,8 +1200,32 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1046,6 +1241,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1403,7 +1610,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="98">
+  <cellXfs count="129">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -1550,40 +1757,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1597,6 +1774,85 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3845,8 +4101,8 @@
   </sheetPr>
   <dimension ref="A1:L57"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5294,16 +5550,16 @@
     <tabColor rgb="FFFFFF00"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:L57"/>
+  <dimension ref="A1:L48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B62" sqref="B62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="38.42578125" style="75" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="64" style="75" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37.85546875" style="75" customWidth="1"/>
     <col min="3" max="3" width="15.28515625" style="75" customWidth="1"/>
     <col min="4" max="4" width="11.85546875" style="75" customWidth="1"/>
     <col min="5" max="5" width="12" style="75" customWidth="1"/>
@@ -5345,7 +5601,7 @@
         <v>20</v>
       </c>
       <c r="B4" s="75" t="s">
-        <v>278</v>
+        <v>350</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -5401,7 +5657,7 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="77" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B9" s="71" t="s">
         <v>48</v>
@@ -5418,667 +5674,668 @@
       <c r="J9" s="71"/>
       <c r="K9" s="72"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="77" t="s">
-        <v>135</v>
-      </c>
-      <c r="B10" s="71" t="s">
-        <v>47</v>
-      </c>
-      <c r="C10" s="71" t="s">
+    <row r="10" spans="1:12" s="113" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="110" t="s">
+        <v>291</v>
+      </c>
+      <c r="B10" s="111" t="s">
+        <v>315</v>
+      </c>
+      <c r="C10" s="108" t="s">
         <v>62</v>
       </c>
-      <c r="D10" s="71"/>
-      <c r="E10" s="71"/>
-      <c r="F10" s="71"/>
-      <c r="G10" s="71" t="s">
-        <v>49</v>
-      </c>
-      <c r="H10" s="71" t="s">
+      <c r="D10" s="108"/>
+      <c r="E10" s="108"/>
+      <c r="F10" s="108"/>
+      <c r="G10" s="108" t="s">
+        <v>49</v>
+      </c>
+      <c r="H10" s="108" t="s">
         <v>50</v>
       </c>
-      <c r="I10" s="71" t="s">
+      <c r="I10" s="108" t="s">
         <v>46</v>
       </c>
-      <c r="J10" s="71"/>
-      <c r="K10" s="78" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="19" t="s">
+      <c r="J10" s="108"/>
+      <c r="K10" s="112" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" s="113" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="110" t="s">
+        <v>348</v>
+      </c>
+      <c r="B11" s="111"/>
+      <c r="C11" s="108" t="s">
+        <v>62</v>
+      </c>
+      <c r="D11" s="108"/>
+      <c r="E11" s="108"/>
+      <c r="F11" s="108"/>
+      <c r="G11" s="108"/>
+      <c r="H11" s="108"/>
+      <c r="I11" s="108"/>
+      <c r="J11" s="108"/>
+      <c r="K11" s="112"/>
+    </row>
+    <row r="12" spans="1:12" s="113" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="110" t="s">
+        <v>292</v>
+      </c>
+      <c r="B12" s="114" t="s">
+        <v>316</v>
+      </c>
+      <c r="C12" s="108" t="s">
+        <v>62</v>
+      </c>
+      <c r="D12" s="108"/>
+      <c r="E12" s="108"/>
+      <c r="F12" s="108"/>
+      <c r="G12" s="108" t="s">
+        <v>49</v>
+      </c>
+      <c r="H12" s="108" t="s">
+        <v>50</v>
+      </c>
+      <c r="I12" s="108" t="s">
+        <v>274</v>
+      </c>
+      <c r="J12" s="108"/>
+      <c r="K12" s="112"/>
+    </row>
+    <row r="13" spans="1:12" s="113" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="115" t="s">
+        <v>293</v>
+      </c>
+      <c r="B13" s="114" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" s="124" t="s">
+        <v>63</v>
+      </c>
+      <c r="D13" s="116">
+        <v>50</v>
+      </c>
+      <c r="E13" s="108"/>
+      <c r="F13" s="108"/>
+      <c r="G13" s="108" t="s">
+        <v>49</v>
+      </c>
+      <c r="H13" s="108" t="s">
+        <v>50</v>
+      </c>
+      <c r="I13" s="108" t="s">
+        <v>293</v>
+      </c>
+      <c r="J13" s="108"/>
+      <c r="K13" s="112"/>
+    </row>
+    <row r="14" spans="1:12" s="113" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="104" t="s">
         <v>70</v>
       </c>
-      <c r="B11" s="19" t="s">
+      <c r="B14" s="104" t="s">
         <v>65</v>
       </c>
-      <c r="C11" s="71" t="s">
+      <c r="C14" s="108" t="s">
         <v>62</v>
       </c>
-      <c r="D11" s="71"/>
-      <c r="E11" s="71"/>
-      <c r="F11" s="71"/>
-      <c r="G11" s="71" t="s">
-        <v>49</v>
-      </c>
-      <c r="H11" s="71" t="s">
+      <c r="D14" s="108"/>
+      <c r="E14" s="108"/>
+      <c r="F14" s="108"/>
+      <c r="G14" s="108" t="s">
+        <v>49</v>
+      </c>
+      <c r="H14" s="108" t="s">
         <v>50</v>
       </c>
-      <c r="I11" s="71" t="s">
+      <c r="I14" s="108" t="s">
         <v>88</v>
       </c>
-      <c r="J11" s="71"/>
-      <c r="K11" s="72" t="s">
+      <c r="J14" s="108"/>
+      <c r="K14" s="112" t="s">
         <v>66</v>
       </c>
-      <c r="L11" s="79"/>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="77" t="s">
+      <c r="L14" s="123"/>
+    </row>
+    <row r="15" spans="1:12" s="113" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="104" t="s">
         <v>136</v>
       </c>
-      <c r="B12" s="77" t="s">
+      <c r="B15" s="104" t="s">
         <v>38</v>
       </c>
-      <c r="C12" s="19" t="s">
+      <c r="C15" s="104" t="s">
         <v>62</v>
       </c>
-      <c r="D12" s="19"/>
-      <c r="E12" s="19"/>
-      <c r="F12" s="71"/>
-      <c r="G12" s="71" t="s">
-        <v>49</v>
-      </c>
-      <c r="H12" s="71" t="s">
+      <c r="D15" s="104"/>
+      <c r="E15" s="104"/>
+      <c r="F15" s="108"/>
+      <c r="G15" s="108" t="s">
+        <v>49</v>
+      </c>
+      <c r="H15" s="108" t="s">
         <v>50</v>
       </c>
-      <c r="I12" s="71" t="s">
+      <c r="I15" s="108" t="s">
         <v>6</v>
       </c>
-      <c r="J12" s="71"/>
-      <c r="K12" s="72" t="s">
+      <c r="J15" s="108"/>
+      <c r="K15" s="112" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" s="21" t="s">
+    <row r="16" spans="1:12" s="113" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="107" t="s">
         <v>137</v>
       </c>
-      <c r="B13" s="21" t="s">
+      <c r="B16" s="107" t="s">
         <v>39</v>
       </c>
-      <c r="C13" s="21" t="s">
+      <c r="C16" s="107" t="s">
         <v>62</v>
       </c>
-      <c r="D13" s="21"/>
-      <c r="E13" s="21"/>
-      <c r="F13" s="21"/>
-      <c r="G13" s="71"/>
-      <c r="H13" s="71"/>
-      <c r="I13" s="21"/>
-      <c r="J13" s="21"/>
-      <c r="K13" s="80" t="s">
+      <c r="D16" s="107"/>
+      <c r="E16" s="107"/>
+      <c r="F16" s="107"/>
+      <c r="G16" s="108"/>
+      <c r="H16" s="108"/>
+      <c r="I16" s="107"/>
+      <c r="J16" s="107"/>
+      <c r="K16" s="125" t="s">
         <v>254</v>
       </c>
-      <c r="L13" s="81"/>
-    </row>
-    <row r="14" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A14" s="21" t="s">
+      <c r="L16" s="126"/>
+    </row>
+    <row r="17" spans="1:11" s="113" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A17" s="107" t="s">
         <v>138</v>
       </c>
-      <c r="B14" s="21" t="s">
+      <c r="B17" s="107" t="s">
         <v>28</v>
       </c>
-      <c r="C14" s="21" t="s">
+      <c r="C17" s="107" t="s">
         <v>62</v>
       </c>
-      <c r="D14" s="21"/>
-      <c r="E14" s="21"/>
-      <c r="F14" s="21"/>
-      <c r="G14" s="71" t="s">
-        <v>49</v>
-      </c>
-      <c r="H14" s="71" t="s">
+      <c r="D17" s="107"/>
+      <c r="E17" s="107"/>
+      <c r="F17" s="107"/>
+      <c r="G17" s="108" t="s">
+        <v>49</v>
+      </c>
+      <c r="H17" s="108" t="s">
         <v>154</v>
       </c>
-      <c r="I14" s="21" t="s">
+      <c r="I17" s="107" t="s">
         <v>253</v>
       </c>
-      <c r="J14" s="21"/>
-      <c r="K14" s="80" t="s">
+      <c r="J17" s="107"/>
+      <c r="K17" s="125" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" s="82" t="s">
+    <row r="18" spans="1:11" s="113" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="107" t="s">
         <v>164</v>
       </c>
-      <c r="B15" s="71" t="s">
+      <c r="B18" s="108" t="s">
         <v>37</v>
       </c>
-      <c r="C15" s="82" t="s">
+      <c r="C18" s="107" t="s">
         <v>62</v>
       </c>
-      <c r="D15" s="71"/>
-      <c r="E15" s="71"/>
-      <c r="F15" s="71"/>
-      <c r="G15" s="71" t="s">
-        <v>49</v>
-      </c>
-      <c r="H15" s="71" t="s">
+      <c r="D18" s="108"/>
+      <c r="E18" s="108"/>
+      <c r="F18" s="108"/>
+      <c r="G18" s="108" t="s">
+        <v>49</v>
+      </c>
+      <c r="H18" s="108" t="s">
         <v>50</v>
       </c>
-      <c r="I15" s="71" t="s">
+      <c r="I18" s="108" t="s">
         <v>51</v>
       </c>
-      <c r="J15" s="71"/>
-      <c r="K15" s="72"/>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" s="82" t="s">
+      <c r="J18" s="108"/>
+      <c r="K18" s="112"/>
+    </row>
+    <row r="19" spans="1:11" s="113" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="107" t="s">
         <v>52</v>
       </c>
-      <c r="B16" s="71" t="s">
+      <c r="B19" s="108" t="s">
         <v>37</v>
       </c>
-      <c r="C16" s="82" t="s">
+      <c r="C19" s="107" t="s">
         <v>62</v>
       </c>
-      <c r="D16" s="71"/>
-      <c r="E16" s="71"/>
-      <c r="F16" s="71"/>
-      <c r="G16" s="71" t="s">
-        <v>49</v>
-      </c>
-      <c r="H16" s="71" t="s">
+      <c r="D19" s="108"/>
+      <c r="E19" s="108"/>
+      <c r="F19" s="108"/>
+      <c r="G19" s="108" t="s">
+        <v>49</v>
+      </c>
+      <c r="H19" s="108" t="s">
         <v>50</v>
       </c>
-      <c r="I16" s="71" t="s">
+      <c r="I19" s="108" t="s">
         <v>53</v>
       </c>
-      <c r="J16" s="71"/>
-      <c r="K16" s="83"/>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="82" t="s">
+      <c r="J19" s="108"/>
+      <c r="K19" s="112"/>
+    </row>
+    <row r="20" spans="1:11" s="113" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="107" t="s">
         <v>165</v>
       </c>
-      <c r="B17" s="71" t="s">
+      <c r="B20" s="108" t="s">
         <v>37</v>
       </c>
-      <c r="C17" s="82" t="s">
+      <c r="C20" s="107" t="s">
         <v>62</v>
       </c>
-      <c r="D17" s="71"/>
-      <c r="E17" s="71"/>
-      <c r="F17" s="71"/>
-      <c r="G17" s="71" t="s">
-        <v>49</v>
-      </c>
-      <c r="H17" s="71" t="s">
+      <c r="D20" s="108"/>
+      <c r="E20" s="108"/>
+      <c r="F20" s="108"/>
+      <c r="G20" s="108" t="s">
+        <v>49</v>
+      </c>
+      <c r="H20" s="108" t="s">
         <v>50</v>
       </c>
-      <c r="I17" s="71" t="s">
+      <c r="I20" s="108" t="s">
         <v>54</v>
       </c>
-      <c r="J17" s="71"/>
-      <c r="K17" s="72"/>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="82" t="s">
-        <v>166</v>
-      </c>
-      <c r="B18" s="71" t="s">
-        <v>37</v>
-      </c>
-      <c r="C18" s="82" t="s">
+      <c r="J20" s="108"/>
+      <c r="K20" s="112"/>
+    </row>
+    <row r="21" spans="1:11" s="113" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="107" t="s">
+        <v>139</v>
+      </c>
+      <c r="B21" s="108"/>
+      <c r="C21" s="107" t="s">
         <v>62</v>
       </c>
-      <c r="D18" s="71"/>
-      <c r="E18" s="71"/>
-      <c r="F18" s="71"/>
-      <c r="G18" s="71" t="s">
-        <v>49</v>
-      </c>
-      <c r="H18" s="71" t="s">
+      <c r="D21" s="108"/>
+      <c r="E21" s="108"/>
+      <c r="F21" s="108"/>
+      <c r="G21" s="108" t="s">
+        <v>49</v>
+      </c>
+      <c r="H21" s="108" t="s">
         <v>50</v>
       </c>
-      <c r="I18" s="71" t="s">
-        <v>60</v>
-      </c>
-      <c r="J18" s="71"/>
-      <c r="K18" s="72"/>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="82" t="s">
-        <v>167</v>
-      </c>
-      <c r="B19" s="71" t="s">
-        <v>37</v>
-      </c>
-      <c r="C19" s="82" t="s">
-        <v>62</v>
-      </c>
-      <c r="D19" s="71"/>
-      <c r="E19" s="71"/>
-      <c r="F19" s="71"/>
-      <c r="G19" s="71" t="s">
-        <v>49</v>
-      </c>
-      <c r="H19" s="71" t="s">
-        <v>154</v>
-      </c>
-      <c r="I19" s="71" t="s">
-        <v>156</v>
-      </c>
-      <c r="J19" s="71"/>
-      <c r="K19" s="72"/>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="82" t="s">
-        <v>168</v>
-      </c>
-      <c r="B20" s="71" t="s">
-        <v>37</v>
-      </c>
-      <c r="C20" s="82" t="s">
-        <v>62</v>
-      </c>
-      <c r="D20" s="71"/>
-      <c r="E20" s="71"/>
-      <c r="F20" s="71"/>
-      <c r="G20" s="71" t="s">
-        <v>49</v>
-      </c>
-      <c r="H20" s="71" t="s">
-        <v>154</v>
-      </c>
-      <c r="I20" s="71" t="s">
-        <v>155</v>
-      </c>
-      <c r="J20" s="71"/>
-      <c r="K20" s="84"/>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="82" t="s">
-        <v>55</v>
-      </c>
-      <c r="B21" s="71"/>
-      <c r="C21" s="82" t="s">
-        <v>64</v>
-      </c>
-      <c r="D21" s="71"/>
-      <c r="E21" s="71"/>
-      <c r="F21" s="71"/>
-      <c r="G21" s="71" t="s">
-        <v>49</v>
-      </c>
-      <c r="H21" s="71" t="s">
+      <c r="I21" s="108" t="s">
+        <v>57</v>
+      </c>
+      <c r="J21" s="108"/>
+      <c r="K21" s="112"/>
+    </row>
+    <row r="22" spans="1:11" s="113" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="107" t="s">
+        <v>140</v>
+      </c>
+      <c r="B22" s="108" t="s">
+        <v>35</v>
+      </c>
+      <c r="C22" s="108" t="s">
+        <v>63</v>
+      </c>
+      <c r="D22" s="108">
+        <v>255</v>
+      </c>
+      <c r="E22" s="108"/>
+      <c r="F22" s="108"/>
+      <c r="G22" s="108" t="s">
+        <v>49</v>
+      </c>
+      <c r="H22" s="108" t="s">
         <v>50</v>
       </c>
-      <c r="I21" s="71" t="s">
-        <v>56</v>
-      </c>
-      <c r="J21" s="71"/>
-      <c r="K21" s="83"/>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="82" t="s">
-        <v>139</v>
-      </c>
-      <c r="B22" s="71"/>
-      <c r="C22" s="82" t="s">
-        <v>62</v>
-      </c>
-      <c r="D22" s="71"/>
-      <c r="E22" s="71"/>
-      <c r="F22" s="71"/>
-      <c r="G22" s="71" t="s">
-        <v>49</v>
-      </c>
-      <c r="H22" s="71" t="s">
+      <c r="I22" s="108" t="s">
+        <v>58</v>
+      </c>
+      <c r="J22" s="108"/>
+      <c r="K22" s="112"/>
+    </row>
+    <row r="23" spans="1:11" s="113" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="108" t="s">
+        <v>141</v>
+      </c>
+      <c r="B23" s="108" t="s">
+        <v>36</v>
+      </c>
+      <c r="C23" s="108" t="s">
+        <v>63</v>
+      </c>
+      <c r="D23" s="108">
         <v>50</v>
       </c>
-      <c r="I22" s="71" t="s">
-        <v>57</v>
-      </c>
-      <c r="J22" s="71"/>
-      <c r="K22" s="72"/>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="82" t="s">
-        <v>140</v>
-      </c>
-      <c r="B23" s="71" t="s">
-        <v>35</v>
-      </c>
-      <c r="C23" s="71" t="s">
+      <c r="E23" s="108"/>
+      <c r="F23" s="108"/>
+      <c r="G23" s="108" t="s">
+        <v>49</v>
+      </c>
+      <c r="H23" s="108" t="s">
+        <v>50</v>
+      </c>
+      <c r="I23" s="108" t="s">
+        <v>5</v>
+      </c>
+      <c r="J23" s="108"/>
+      <c r="K23" s="108"/>
+    </row>
+    <row r="24" spans="1:11" s="113" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="107" t="s">
+        <v>142</v>
+      </c>
+      <c r="B24" s="108"/>
+      <c r="C24" s="107" t="s">
         <v>63</v>
       </c>
-      <c r="D23" s="71">
-        <v>20</v>
-      </c>
-      <c r="E23" s="71"/>
-      <c r="F23" s="71"/>
-      <c r="G23" s="71" t="s">
-        <v>49</v>
-      </c>
-      <c r="H23" s="71" t="s">
+      <c r="D24" s="108">
         <v>50</v>
       </c>
-      <c r="I23" s="71" t="s">
+      <c r="E24" s="108"/>
+      <c r="F24" s="108"/>
+      <c r="G24" s="108" t="s">
+        <v>49</v>
+      </c>
+      <c r="H24" s="108" t="s">
+        <v>50</v>
+      </c>
+      <c r="I24" s="108" t="s">
+        <v>89</v>
+      </c>
+      <c r="J24" s="108"/>
+      <c r="K24" s="108"/>
+    </row>
+    <row r="25" spans="1:11" s="113" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="108" t="s">
+        <v>256</v>
+      </c>
+      <c r="B25" s="108"/>
+      <c r="C25" s="109" t="s">
+        <v>284</v>
+      </c>
+      <c r="D25" s="127" t="s">
+        <v>285</v>
+      </c>
+      <c r="E25" s="108"/>
+      <c r="F25" s="108"/>
+      <c r="G25" s="127" t="s">
+        <v>49</v>
+      </c>
+      <c r="H25" s="108" t="s">
+        <v>50</v>
+      </c>
+      <c r="I25" s="127" t="s">
+        <v>256</v>
+      </c>
+      <c r="J25" s="108"/>
+      <c r="K25" s="108"/>
+    </row>
+    <row r="26" spans="1:11" s="113" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="116" t="s">
+        <v>298</v>
+      </c>
+      <c r="B26" s="114" t="s">
+        <v>321</v>
+      </c>
+      <c r="C26" s="109" t="s">
+        <v>63</v>
+      </c>
+      <c r="D26" s="108">
+        <v>8000</v>
+      </c>
+      <c r="E26" s="108"/>
+      <c r="F26" s="108"/>
+      <c r="G26" s="108" t="s">
+        <v>49</v>
+      </c>
+      <c r="H26" s="116" t="s">
+        <v>340</v>
+      </c>
+      <c r="I26" s="116" t="s">
+        <v>298</v>
+      </c>
+      <c r="J26" s="108"/>
+      <c r="K26" s="112"/>
+    </row>
+    <row r="27" spans="1:11" s="113" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="115" t="s">
+        <v>299</v>
+      </c>
+      <c r="B27" s="114" t="s">
+        <v>322</v>
+      </c>
+      <c r="C27" s="109" t="s">
+        <v>63</v>
+      </c>
+      <c r="D27" s="127">
+        <v>100</v>
+      </c>
+      <c r="E27" s="108"/>
+      <c r="F27" s="108"/>
+      <c r="G27" s="108" t="s">
+        <v>49</v>
+      </c>
+      <c r="H27" s="116" t="s">
+        <v>340</v>
+      </c>
+      <c r="I27" s="115" t="s">
+        <v>299</v>
+      </c>
+      <c r="J27" s="108"/>
+      <c r="K27" s="112"/>
+    </row>
+    <row r="28" spans="1:11" s="113" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="115" t="s">
+        <v>300</v>
+      </c>
+      <c r="B28" s="114" t="s">
+        <v>6</v>
+      </c>
+      <c r="C28" s="107" t="s">
+        <v>63</v>
+      </c>
+      <c r="D28" s="108">
+        <v>50</v>
+      </c>
+      <c r="E28" s="108"/>
+      <c r="F28" s="108"/>
+      <c r="G28" s="108" t="s">
+        <v>49</v>
+      </c>
+      <c r="H28" s="116" t="s">
+        <v>340</v>
+      </c>
+      <c r="I28" s="115" t="s">
+        <v>300</v>
+      </c>
+      <c r="J28" s="108"/>
+      <c r="K28" s="112"/>
+    </row>
+    <row r="29" spans="1:11" s="123" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="119" t="s">
+        <v>307</v>
+      </c>
+      <c r="B29" s="119" t="s">
+        <v>329</v>
+      </c>
+      <c r="C29" s="128" t="s">
+        <v>63</v>
+      </c>
+      <c r="D29" s="128">
+        <v>255</v>
+      </c>
+      <c r="E29" s="120"/>
+      <c r="F29" s="120"/>
+      <c r="G29" s="120" t="s">
+        <v>49</v>
+      </c>
+      <c r="H29" s="121" t="s">
+        <v>340</v>
+      </c>
+      <c r="I29" s="120" t="s">
         <v>58</v>
       </c>
-      <c r="J23" s="71"/>
-      <c r="K23" s="72"/>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="71" t="s">
-        <v>141</v>
-      </c>
-      <c r="B24" s="71" t="s">
-        <v>36</v>
-      </c>
-      <c r="C24" s="71" t="s">
+      <c r="J29" s="120"/>
+      <c r="K29" s="122"/>
+    </row>
+    <row r="30" spans="1:11" s="113" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="115" t="s">
+        <v>308</v>
+      </c>
+      <c r="B30" s="114" t="s">
+        <v>332</v>
+      </c>
+      <c r="C30" s="109" t="s">
         <v>63</v>
       </c>
-      <c r="D24" s="71">
-        <v>20</v>
-      </c>
-      <c r="E24" s="71"/>
-      <c r="F24" s="71"/>
-      <c r="G24" s="71" t="s">
-        <v>49</v>
-      </c>
-      <c r="H24" s="71" t="s">
-        <v>50</v>
-      </c>
-      <c r="I24" s="71" t="s">
-        <v>5</v>
-      </c>
-      <c r="J24" s="71"/>
-      <c r="K24" s="71"/>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" s="82" t="s">
-        <v>142</v>
-      </c>
-      <c r="B25" s="71"/>
-      <c r="C25" s="82" t="s">
+      <c r="D30" s="127">
+        <v>5000</v>
+      </c>
+      <c r="E30" s="108"/>
+      <c r="F30" s="108"/>
+      <c r="G30" s="108" t="s">
+        <v>49</v>
+      </c>
+      <c r="H30" s="116" t="s">
+        <v>340</v>
+      </c>
+      <c r="I30" s="108" t="s">
+        <v>308</v>
+      </c>
+      <c r="J30" s="108"/>
+      <c r="K30" s="112"/>
+    </row>
+    <row r="31" spans="1:11" s="113" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="110" t="s">
+        <v>313</v>
+      </c>
+      <c r="B31" s="114" t="s">
+        <v>313</v>
+      </c>
+      <c r="C31" s="109" t="s">
         <v>63</v>
       </c>
-      <c r="D25" s="84">
-        <v>50</v>
-      </c>
-      <c r="E25" s="71"/>
-      <c r="F25" s="71"/>
-      <c r="G25" s="71" t="s">
-        <v>49</v>
-      </c>
-      <c r="H25" s="71" t="s">
-        <v>50</v>
-      </c>
-      <c r="I25" s="84" t="s">
-        <v>89</v>
-      </c>
-      <c r="J25" s="71"/>
-      <c r="K25" s="71"/>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" s="82" t="s">
-        <v>238</v>
-      </c>
-      <c r="B26" s="71" t="s">
-        <v>239</v>
-      </c>
-      <c r="C26" s="82" t="s">
+      <c r="D31" s="108">
+        <v>8000</v>
+      </c>
+      <c r="E31" s="108"/>
+      <c r="F31" s="108"/>
+      <c r="G31" s="108" t="s">
+        <v>49</v>
+      </c>
+      <c r="H31" s="116" t="s">
+        <v>340</v>
+      </c>
+      <c r="I31" s="110" t="s">
+        <v>313</v>
+      </c>
+      <c r="J31" s="108"/>
+      <c r="K31" s="116" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A32" s="115" t="s">
+        <v>294</v>
+      </c>
+      <c r="B32" s="89" t="s">
+        <v>317</v>
+      </c>
+      <c r="C32" s="80" t="s">
         <v>63</v>
       </c>
-      <c r="D26" s="84">
-        <v>50</v>
-      </c>
-      <c r="E26" s="71"/>
-      <c r="F26" s="71"/>
-      <c r="G26" s="71" t="s">
-        <v>49</v>
-      </c>
-      <c r="H26" s="71" t="s">
-        <v>50</v>
-      </c>
-      <c r="I26" s="84" t="s">
-        <v>3</v>
-      </c>
-      <c r="J26" s="71"/>
-      <c r="K26" s="71" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" s="82" t="s">
-        <v>145</v>
-      </c>
-      <c r="B27" s="71"/>
-      <c r="C27" s="82" t="s">
-        <v>63</v>
-      </c>
-      <c r="D27" s="84">
-        <v>50</v>
-      </c>
-      <c r="E27" s="71"/>
-      <c r="F27" s="71"/>
-      <c r="G27" s="71" t="s">
-        <v>49</v>
-      </c>
-      <c r="H27" s="71" t="s">
-        <v>50</v>
-      </c>
-      <c r="I27" s="84" t="s">
-        <v>91</v>
-      </c>
-      <c r="J27" s="71"/>
-      <c r="K27" s="71" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" s="82" t="s">
-        <v>143</v>
-      </c>
-      <c r="B28" s="71"/>
-      <c r="C28" s="82" t="s">
-        <v>63</v>
-      </c>
-      <c r="D28" s="84">
-        <v>3</v>
-      </c>
-      <c r="E28" s="71" t="s">
-        <v>93</v>
-      </c>
-      <c r="F28" s="71"/>
-      <c r="G28" s="71" t="s">
-        <v>49</v>
-      </c>
-      <c r="H28" s="71" t="s">
-        <v>50</v>
-      </c>
-      <c r="I28" s="84" t="s">
-        <v>92</v>
-      </c>
-      <c r="J28" s="71"/>
-      <c r="K28" s="71" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" s="82" t="s">
-        <v>144</v>
-      </c>
-      <c r="B29" s="71"/>
-      <c r="C29" s="82" t="s">
-        <v>63</v>
-      </c>
-      <c r="D29" s="84">
-        <v>3</v>
-      </c>
-      <c r="E29" s="71" t="s">
-        <v>93</v>
-      </c>
-      <c r="F29" s="71"/>
-      <c r="G29" s="71" t="s">
-        <v>49</v>
-      </c>
-      <c r="H29" s="71" t="s">
-        <v>50</v>
-      </c>
-      <c r="I29" s="84" t="s">
-        <v>96</v>
-      </c>
-      <c r="J29" s="71"/>
-      <c r="K29" s="71" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A30" s="82" t="s">
-        <v>94</v>
-      </c>
-      <c r="B30" s="71"/>
-      <c r="C30" s="82" t="s">
-        <v>63</v>
-      </c>
-      <c r="D30" s="84">
-        <v>3</v>
-      </c>
-      <c r="E30" s="71" t="s">
-        <v>93</v>
-      </c>
-      <c r="F30" s="71"/>
-      <c r="G30" s="71" t="s">
-        <v>49</v>
-      </c>
-      <c r="H30" s="71" t="s">
-        <v>50</v>
-      </c>
-      <c r="I30" s="84" t="s">
-        <v>97</v>
-      </c>
-      <c r="J30" s="71"/>
-      <c r="K30" s="71" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A31" s="82" t="s">
-        <v>95</v>
-      </c>
-      <c r="B31" s="71"/>
-      <c r="C31" s="82" t="s">
-        <v>63</v>
-      </c>
-      <c r="D31" s="84">
-        <v>3</v>
-      </c>
-      <c r="E31" s="71" t="s">
-        <v>93</v>
-      </c>
-      <c r="F31" s="71"/>
-      <c r="G31" s="71" t="s">
-        <v>49</v>
-      </c>
-      <c r="H31" s="71" t="s">
-        <v>50</v>
-      </c>
-      <c r="I31" s="84" t="s">
-        <v>98</v>
-      </c>
-      <c r="J31" s="71"/>
-      <c r="K31" s="71"/>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A32" s="82" t="s">
-        <v>100</v>
-      </c>
-      <c r="B32" s="71"/>
-      <c r="C32" s="82" t="s">
-        <v>63</v>
-      </c>
-      <c r="D32" s="84">
-        <v>20</v>
+      <c r="D32" s="81">
+        <v>255</v>
       </c>
       <c r="E32" s="71"/>
       <c r="F32" s="71"/>
       <c r="G32" s="71" t="s">
         <v>49</v>
       </c>
-      <c r="H32" s="71" t="s">
-        <v>50</v>
-      </c>
-      <c r="I32" s="84" t="s">
-        <v>101</v>
-      </c>
-      <c r="J32" s="71"/>
-      <c r="K32" s="71"/>
+      <c r="H32" s="91" t="s">
+        <v>338</v>
+      </c>
+      <c r="I32" s="92" t="s">
+        <v>294</v>
+      </c>
+      <c r="K32" s="91" t="s">
+        <v>339</v>
+      </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A33" s="82" t="s">
-        <v>102</v>
-      </c>
-      <c r="B33" s="71"/>
-      <c r="C33" s="82" t="s">
+      <c r="A33" s="115" t="s">
+        <v>295</v>
+      </c>
+      <c r="B33" s="90" t="s">
+        <v>318</v>
+      </c>
+      <c r="C33" s="71" t="s">
         <v>63</v>
       </c>
-      <c r="D33" s="84">
-        <v>20</v>
+      <c r="D33" s="71">
+        <v>3</v>
       </c>
       <c r="E33" s="71"/>
       <c r="F33" s="71"/>
       <c r="G33" s="71" t="s">
         <v>49</v>
       </c>
-      <c r="H33" s="71" t="s">
-        <v>50</v>
-      </c>
-      <c r="I33" s="84" t="s">
-        <v>103</v>
-      </c>
-      <c r="J33" s="71"/>
-      <c r="K33" s="71"/>
+      <c r="H33" s="91" t="s">
+        <v>338</v>
+      </c>
+      <c r="I33" s="92" t="s">
+        <v>295</v>
+      </c>
+      <c r="K33" s="91" t="s">
+        <v>339</v>
+      </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A34" s="82" t="s">
-        <v>104</v>
-      </c>
-      <c r="B34" s="71"/>
-      <c r="C34" s="82" t="s">
+      <c r="A34" s="115" t="s">
+        <v>296</v>
+      </c>
+      <c r="B34" s="90" t="s">
+        <v>319</v>
+      </c>
+      <c r="C34" s="71" t="s">
         <v>63</v>
       </c>
-      <c r="D34" s="84">
-        <v>50</v>
+      <c r="D34" s="71">
+        <v>3</v>
       </c>
       <c r="E34" s="71"/>
       <c r="F34" s="71"/>
       <c r="G34" s="71" t="s">
         <v>49</v>
       </c>
-      <c r="H34" s="71" t="s">
-        <v>50</v>
-      </c>
-      <c r="I34" s="84" t="s">
-        <v>105</v>
-      </c>
-      <c r="J34" s="71"/>
-      <c r="K34" s="71"/>
+      <c r="H34" s="91" t="s">
+        <v>338</v>
+      </c>
+      <c r="I34" s="92" t="s">
+        <v>296</v>
+      </c>
+      <c r="K34" s="91" t="s">
+        <v>339</v>
+      </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A35" s="82" t="s">
-        <v>106</v>
-      </c>
-      <c r="B35" s="71"/>
-      <c r="C35" s="82" t="s">
+      <c r="A35" s="115" t="s">
+        <v>297</v>
+      </c>
+      <c r="B35" s="89" t="s">
+        <v>320</v>
+      </c>
+      <c r="C35" s="71" t="s">
         <v>63</v>
       </c>
-      <c r="D35" s="84">
-        <v>50</v>
+      <c r="D35" s="71">
+        <v>3</v>
       </c>
       <c r="E35" s="71"/>
       <c r="F35" s="71"/>
@@ -6086,649 +6343,367 @@
         <v>49</v>
       </c>
       <c r="H35" s="71" t="s">
+        <v>338</v>
+      </c>
+      <c r="I35" s="92" t="s">
+        <v>297</v>
+      </c>
+      <c r="J35" s="71"/>
+      <c r="K35" s="93" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A36" s="115" t="s">
+        <v>301</v>
+      </c>
+      <c r="B36" s="89" t="s">
+        <v>323</v>
+      </c>
+      <c r="C36" s="71" t="s">
+        <v>63</v>
+      </c>
+      <c r="D36" s="71">
         <v>50</v>
-      </c>
-      <c r="I35" s="84" t="s">
-        <v>107</v>
-      </c>
-      <c r="J35" s="71"/>
-      <c r="K35" s="84"/>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A36" s="82" t="s">
-        <v>146</v>
-      </c>
-      <c r="B36" s="71"/>
-      <c r="C36" s="82" t="s">
-        <v>63</v>
-      </c>
-      <c r="D36" s="71">
-        <v>255</v>
       </c>
       <c r="E36" s="71"/>
       <c r="F36" s="71"/>
       <c r="G36" s="71" t="s">
         <v>49</v>
       </c>
-      <c r="H36" s="71" t="s">
-        <v>50</v>
-      </c>
-      <c r="I36" s="84" t="s">
-        <v>169</v>
+      <c r="H36" s="94" t="s">
+        <v>341</v>
+      </c>
+      <c r="I36" s="95" t="s">
+        <v>301</v>
       </c>
       <c r="J36" s="71"/>
-      <c r="K36" s="84" t="s">
-        <v>149</v>
+      <c r="K36" s="96" t="s">
+        <v>342</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A37" s="82" t="s">
-        <v>147</v>
-      </c>
-      <c r="B37" s="71"/>
-      <c r="C37" s="82" t="s">
+      <c r="A37" s="115" t="s">
+        <v>302</v>
+      </c>
+      <c r="B37" s="89" t="s">
+        <v>324</v>
+      </c>
+      <c r="C37" s="71" t="s">
         <v>63</v>
       </c>
-      <c r="D37" s="84">
-        <v>3</v>
-      </c>
-      <c r="E37" s="71" t="s">
-        <v>93</v>
-      </c>
+      <c r="D37" s="71">
+        <v>200</v>
+      </c>
+      <c r="E37" s="71"/>
       <c r="F37" s="71"/>
       <c r="G37" s="71" t="s">
         <v>49</v>
       </c>
-      <c r="H37" s="71" t="s">
-        <v>50</v>
-      </c>
-      <c r="I37" s="71" t="s">
-        <v>148</v>
+      <c r="H37" s="94" t="s">
+        <v>341</v>
+      </c>
+      <c r="I37" s="95" t="s">
+        <v>302</v>
       </c>
       <c r="J37" s="71"/>
-      <c r="K37" s="71" t="s">
-        <v>99</v>
+      <c r="K37" s="96" t="s">
+        <v>342</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A38" s="82" t="s">
-        <v>150</v>
-      </c>
-      <c r="B38" s="71"/>
-      <c r="C38" s="82" t="s">
+      <c r="A38" s="115" t="s">
+        <v>303</v>
+      </c>
+      <c r="B38" s="89" t="s">
+        <v>325</v>
+      </c>
+      <c r="C38" s="71" t="s">
         <v>63</v>
       </c>
-      <c r="D38" s="84">
+      <c r="D38" s="71">
         <v>3</v>
       </c>
-      <c r="E38" s="71" t="s">
-        <v>93</v>
-      </c>
+      <c r="E38" s="71"/>
       <c r="F38" s="71"/>
       <c r="G38" s="71" t="s">
         <v>49</v>
       </c>
-      <c r="H38" s="71" t="s">
-        <v>154</v>
-      </c>
-      <c r="I38" s="71" t="s">
-        <v>157</v>
+      <c r="H38" s="94" t="s">
+        <v>341</v>
+      </c>
+      <c r="I38" s="95" t="s">
+        <v>303</v>
       </c>
       <c r="J38" s="71"/>
-      <c r="K38" s="71" t="s">
-        <v>99</v>
+      <c r="K38" s="96" t="s">
+        <v>342</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A39" s="82" t="s">
-        <v>151</v>
-      </c>
-      <c r="B39" s="71"/>
-      <c r="C39" s="82" t="s">
+      <c r="A39" s="115" t="s">
+        <v>304</v>
+      </c>
+      <c r="B39" s="89" t="s">
+        <v>326</v>
+      </c>
+      <c r="C39" s="71" t="s">
         <v>63</v>
       </c>
-      <c r="D39" s="84">
-        <v>3</v>
-      </c>
-      <c r="E39" s="71" t="s">
-        <v>93</v>
-      </c>
+      <c r="D39" s="71">
+        <v>50</v>
+      </c>
+      <c r="E39" s="71"/>
       <c r="F39" s="71"/>
       <c r="G39" s="71" t="s">
         <v>49</v>
       </c>
-      <c r="H39" s="71" t="s">
-        <v>50</v>
-      </c>
-      <c r="I39" s="71" t="s">
-        <v>158</v>
+      <c r="H39" s="94" t="s">
+        <v>341</v>
+      </c>
+      <c r="I39" s="95" t="s">
+        <v>304</v>
       </c>
       <c r="J39" s="71"/>
-      <c r="K39" s="71" t="s">
-        <v>99</v>
+      <c r="K39" s="96" t="s">
+        <v>342</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A40" s="82" t="s">
-        <v>152</v>
-      </c>
-      <c r="B40" s="71"/>
-      <c r="C40" s="82" t="s">
-        <v>63</v>
-      </c>
-      <c r="D40" s="84">
-        <v>3</v>
-      </c>
-      <c r="E40" s="71" t="s">
-        <v>93</v>
-      </c>
+      <c r="A40" s="115" t="s">
+        <v>305</v>
+      </c>
+      <c r="B40" s="89" t="s">
+        <v>327</v>
+      </c>
+      <c r="C40" s="71" t="s">
+        <v>64</v>
+      </c>
+      <c r="D40" s="71"/>
+      <c r="E40" s="71"/>
       <c r="F40" s="71"/>
       <c r="G40" s="71" t="s">
         <v>49</v>
       </c>
-      <c r="H40" s="71" t="s">
-        <v>50</v>
-      </c>
-      <c r="I40" s="71" t="s">
-        <v>153</v>
+      <c r="H40" s="97" t="s">
+        <v>338</v>
+      </c>
+      <c r="I40" s="98" t="s">
+        <v>305</v>
       </c>
       <c r="J40" s="71"/>
-      <c r="K40" s="84"/>
+      <c r="K40" s="99" t="s">
+        <v>339</v>
+      </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A41" s="82" t="s">
-        <v>163</v>
-      </c>
-      <c r="B41" s="71"/>
-      <c r="C41" s="82" t="s">
-        <v>63</v>
-      </c>
-      <c r="D41" s="84">
-        <v>3</v>
-      </c>
-      <c r="E41" s="71" t="s">
-        <v>93</v>
-      </c>
+      <c r="A41" s="115" t="s">
+        <v>306</v>
+      </c>
+      <c r="B41" s="89" t="s">
+        <v>328</v>
+      </c>
+      <c r="C41" s="71" t="s">
+        <v>64</v>
+      </c>
+      <c r="D41" s="71"/>
+      <c r="E41" s="71"/>
       <c r="F41" s="71"/>
       <c r="G41" s="71" t="s">
         <v>49</v>
       </c>
-      <c r="H41" s="84" t="s">
-        <v>159</v>
-      </c>
-      <c r="I41" s="84" t="s">
-        <v>160</v>
+      <c r="H41" s="97" t="s">
+        <v>338</v>
+      </c>
+      <c r="I41" s="98" t="s">
+        <v>306</v>
       </c>
       <c r="J41" s="71"/>
-      <c r="K41" s="71" t="s">
-        <v>99</v>
+      <c r="K41" s="99" t="s">
+        <v>339</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A42" s="85" t="s">
-        <v>170</v>
-      </c>
-      <c r="B42" s="86" t="s">
-        <v>171</v>
-      </c>
-      <c r="C42" s="85" t="s">
+      <c r="A42" s="117" t="s">
+        <v>330</v>
+      </c>
+      <c r="B42" s="118" t="s">
+        <v>330</v>
+      </c>
+      <c r="C42" s="71"/>
+      <c r="D42" s="71"/>
+      <c r="E42" s="71"/>
+      <c r="F42" s="71"/>
+      <c r="G42" s="71"/>
+      <c r="H42" s="71"/>
+      <c r="I42" s="71"/>
+      <c r="J42" s="71"/>
+      <c r="K42" s="78" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A43" s="117" t="s">
+        <v>331</v>
+      </c>
+      <c r="B43" s="118" t="s">
+        <v>331</v>
+      </c>
+      <c r="C43" s="71"/>
+      <c r="D43" s="71"/>
+      <c r="E43" s="71"/>
+      <c r="F43" s="71"/>
+      <c r="G43" s="71"/>
+      <c r="H43" s="71"/>
+      <c r="I43" s="71"/>
+      <c r="J43" s="71"/>
+      <c r="K43" s="78" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A44" s="119" t="s">
+        <v>309</v>
+      </c>
+      <c r="B44" s="88" t="s">
+        <v>333</v>
+      </c>
+      <c r="C44" s="102" t="s">
         <v>63</v>
       </c>
-      <c r="D42" s="86">
+      <c r="D44" s="102">
+        <v>500</v>
+      </c>
+      <c r="E44" s="102"/>
+      <c r="F44" s="102"/>
+      <c r="G44" s="102" t="s">
+        <v>49</v>
+      </c>
+      <c r="H44" s="103" t="s">
+        <v>343</v>
+      </c>
+      <c r="I44" s="100" t="s">
+        <v>309</v>
+      </c>
+      <c r="J44" s="102"/>
+      <c r="K44" s="103" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A45" s="119" t="s">
+        <v>310</v>
+      </c>
+      <c r="B45" s="100" t="s">
+        <v>334</v>
+      </c>
+      <c r="C45" s="102" t="s">
+        <v>63</v>
+      </c>
+      <c r="D45" s="102">
         <v>3</v>
       </c>
-      <c r="E42" s="86" t="s">
-        <v>93</v>
-      </c>
-      <c r="F42" s="86"/>
-      <c r="G42" s="86" t="s">
-        <v>49</v>
-      </c>
-      <c r="H42" s="86" t="s">
-        <v>172</v>
-      </c>
-      <c r="I42" s="86" t="s">
-        <v>173</v>
-      </c>
-      <c r="J42" s="86"/>
-      <c r="K42" s="86" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A43" s="85" t="s">
-        <v>174</v>
-      </c>
-      <c r="B43" s="86" t="s">
-        <v>175</v>
-      </c>
-      <c r="C43" s="85" t="s">
+      <c r="E45" s="102"/>
+      <c r="F45" s="102"/>
+      <c r="G45" s="102" t="s">
+        <v>49</v>
+      </c>
+      <c r="H45" s="103" t="s">
+        <v>343</v>
+      </c>
+      <c r="I45" s="100" t="s">
+        <v>310</v>
+      </c>
+      <c r="J45" s="102"/>
+      <c r="K45" s="103" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A46" s="119" t="s">
+        <v>311</v>
+      </c>
+      <c r="B46" s="100" t="s">
+        <v>335</v>
+      </c>
+      <c r="C46" s="102" t="s">
         <v>63</v>
       </c>
-      <c r="D43" s="86">
+      <c r="D46" s="102">
+        <v>100</v>
+      </c>
+      <c r="E46" s="102"/>
+      <c r="F46" s="102"/>
+      <c r="G46" s="102" t="s">
+        <v>49</v>
+      </c>
+      <c r="H46" s="103" t="s">
+        <v>343</v>
+      </c>
+      <c r="I46" s="100" t="s">
+        <v>311</v>
+      </c>
+      <c r="J46" s="102"/>
+      <c r="K46" s="103" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A47" s="110" t="s">
+        <v>312</v>
+      </c>
+      <c r="B47" s="90" t="s">
+        <v>336</v>
+      </c>
+      <c r="C47" s="71" t="s">
+        <v>63</v>
+      </c>
+      <c r="D47" s="71">
         <v>3</v>
       </c>
-      <c r="E43" s="86" t="s">
-        <v>93</v>
-      </c>
-      <c r="F43" s="86"/>
-      <c r="G43" s="86" t="s">
-        <v>49</v>
-      </c>
-      <c r="H43" s="86" t="s">
-        <v>172</v>
-      </c>
-      <c r="I43" s="86" t="s">
-        <v>176</v>
-      </c>
-      <c r="J43" s="86"/>
-      <c r="K43" s="86" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A44" s="85" t="s">
-        <v>177</v>
-      </c>
-      <c r="B44" s="86" t="s">
-        <v>178</v>
-      </c>
-      <c r="C44" s="85" t="s">
+      <c r="E47" s="71"/>
+      <c r="F47" s="71"/>
+      <c r="G47" s="71" t="s">
+        <v>49</v>
+      </c>
+      <c r="H47" s="101" t="s">
+        <v>344</v>
+      </c>
+      <c r="I47" s="105" t="s">
+        <v>312</v>
+      </c>
+      <c r="J47" s="71"/>
+      <c r="K47" s="106" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" s="79" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="121" t="s">
+        <v>314</v>
+      </c>
+      <c r="B48" s="88" t="s">
+        <v>337</v>
+      </c>
+      <c r="C48" s="102" t="s">
         <v>63</v>
       </c>
-      <c r="D44" s="86">
-        <v>3</v>
-      </c>
-      <c r="E44" s="86" t="s">
-        <v>93</v>
-      </c>
-      <c r="F44" s="86"/>
-      <c r="G44" s="86" t="s">
-        <v>49</v>
-      </c>
-      <c r="H44" s="86" t="s">
-        <v>172</v>
-      </c>
-      <c r="I44" s="86" t="s">
-        <v>179</v>
-      </c>
-      <c r="J44" s="86"/>
-      <c r="K44" s="86" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A45" s="85" t="s">
-        <v>180</v>
-      </c>
-      <c r="B45" s="86" t="s">
-        <v>181</v>
-      </c>
-      <c r="C45" s="85" t="s">
-        <v>63</v>
-      </c>
-      <c r="D45" s="86">
-        <v>3</v>
-      </c>
-      <c r="E45" s="86" t="s">
-        <v>93</v>
-      </c>
-      <c r="F45" s="86"/>
-      <c r="G45" s="86" t="s">
-        <v>49</v>
-      </c>
-      <c r="H45" s="86" t="s">
-        <v>182</v>
-      </c>
-      <c r="I45" s="86" t="s">
-        <v>183</v>
-      </c>
-      <c r="J45" s="86"/>
-      <c r="K45" s="86" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A46" s="85" t="s">
-        <v>184</v>
-      </c>
-      <c r="B46" s="86" t="s">
-        <v>185</v>
-      </c>
-      <c r="C46" s="85" t="s">
-        <v>63</v>
-      </c>
-      <c r="D46" s="86">
-        <v>3</v>
-      </c>
-      <c r="E46" s="86" t="s">
-        <v>93</v>
-      </c>
-      <c r="F46" s="86"/>
-      <c r="G46" s="86" t="s">
-        <v>49</v>
-      </c>
-      <c r="H46" s="86" t="s">
-        <v>154</v>
-      </c>
-      <c r="I46" s="86" t="s">
-        <v>186</v>
-      </c>
-      <c r="J46" s="86"/>
-      <c r="K46" s="86" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A47" s="85" t="s">
-        <v>187</v>
-      </c>
-      <c r="B47" s="86" t="s">
-        <v>188</v>
-      </c>
-      <c r="C47" s="85" t="s">
-        <v>63</v>
-      </c>
-      <c r="D47" s="86">
-        <v>3</v>
-      </c>
-      <c r="E47" s="86" t="s">
-        <v>93</v>
-      </c>
-      <c r="F47" s="86"/>
-      <c r="G47" s="86" t="s">
-        <v>49</v>
-      </c>
-      <c r="H47" s="86" t="s">
-        <v>154</v>
-      </c>
-      <c r="I47" s="86" t="s">
-        <v>189</v>
-      </c>
-      <c r="J47" s="86"/>
-      <c r="K47" s="86" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A48" s="85" t="s">
-        <v>190</v>
-      </c>
-      <c r="B48" s="86" t="s">
-        <v>191</v>
-      </c>
-      <c r="C48" s="85" t="s">
-        <v>63</v>
-      </c>
-      <c r="D48" s="86">
-        <v>3</v>
-      </c>
-      <c r="E48" s="86" t="s">
-        <v>93</v>
-      </c>
-      <c r="F48" s="86"/>
-      <c r="G48" s="86" t="s">
-        <v>49</v>
-      </c>
-      <c r="H48" s="86" t="s">
-        <v>172</v>
-      </c>
-      <c r="I48" s="86" t="s">
-        <v>192</v>
-      </c>
-      <c r="J48" s="86"/>
-      <c r="K48" s="86" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A49" s="85" t="s">
-        <v>193</v>
-      </c>
-      <c r="B49" s="86" t="s">
-        <v>194</v>
-      </c>
-      <c r="C49" s="85" t="s">
-        <v>63</v>
-      </c>
-      <c r="D49" s="86">
-        <v>3</v>
-      </c>
-      <c r="E49" s="86" t="s">
-        <v>93</v>
-      </c>
-      <c r="F49" s="86"/>
-      <c r="G49" s="86" t="s">
-        <v>49</v>
-      </c>
-      <c r="H49" s="86" t="s">
-        <v>172</v>
-      </c>
-      <c r="I49" s="86" t="s">
-        <v>195</v>
-      </c>
-      <c r="J49" s="86"/>
-      <c r="K49" s="86" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A50" s="85" t="s">
-        <v>196</v>
-      </c>
-      <c r="B50" s="86" t="s">
-        <v>197</v>
-      </c>
-      <c r="C50" s="85" t="s">
-        <v>63</v>
-      </c>
-      <c r="D50" s="86">
-        <v>3</v>
-      </c>
-      <c r="E50" s="86" t="s">
-        <v>93</v>
-      </c>
-      <c r="F50" s="86"/>
-      <c r="G50" s="86" t="s">
-        <v>49</v>
-      </c>
-      <c r="H50" s="86" t="s">
-        <v>172</v>
-      </c>
-      <c r="I50" s="86" t="s">
-        <v>198</v>
-      </c>
-      <c r="J50" s="86"/>
-      <c r="K50" s="86" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A51" s="85" t="s">
-        <v>199</v>
-      </c>
-      <c r="B51" s="86" t="s">
-        <v>200</v>
-      </c>
-      <c r="C51" s="85" t="s">
-        <v>63</v>
-      </c>
-      <c r="D51" s="86">
-        <v>3</v>
-      </c>
-      <c r="E51" s="86" t="s">
-        <v>93</v>
-      </c>
-      <c r="F51" s="86"/>
-      <c r="G51" s="86" t="s">
-        <v>49</v>
-      </c>
-      <c r="H51" s="86" t="s">
-        <v>172</v>
-      </c>
-      <c r="I51" s="86" t="s">
-        <v>201</v>
-      </c>
-      <c r="J51" s="86"/>
-      <c r="K51" s="86" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A52" s="87" t="s">
-        <v>209</v>
-      </c>
-      <c r="B52" s="71" t="s">
-        <v>208</v>
-      </c>
-      <c r="C52" s="87" t="s">
-        <v>63</v>
-      </c>
-      <c r="D52" s="88">
-        <v>3</v>
-      </c>
-      <c r="E52" s="88" t="s">
-        <v>93</v>
-      </c>
-      <c r="F52" s="71"/>
-      <c r="G52" s="88" t="s">
-        <v>49</v>
-      </c>
-      <c r="H52" s="86" t="s">
-        <v>172</v>
-      </c>
-      <c r="I52" s="71" t="s">
-        <v>210</v>
-      </c>
-      <c r="J52" s="71"/>
-      <c r="K52" s="86" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A53" s="71" t="s">
-        <v>256</v>
-      </c>
-      <c r="B53" s="71"/>
-      <c r="C53" s="87" t="s">
-        <v>63</v>
-      </c>
-      <c r="D53" s="88">
-        <v>255</v>
-      </c>
-      <c r="E53" s="71"/>
-      <c r="F53" s="71"/>
-      <c r="G53" s="88" t="s">
-        <v>49</v>
-      </c>
-      <c r="H53" s="71" t="s">
-        <v>50</v>
-      </c>
-      <c r="I53" s="88" t="s">
-        <v>256</v>
-      </c>
-      <c r="J53" s="71"/>
-      <c r="K53" s="71"/>
-    </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A54" s="87" t="s">
-        <v>257</v>
-      </c>
-      <c r="B54" s="71"/>
-      <c r="C54" s="87" t="s">
-        <v>63</v>
-      </c>
-      <c r="D54" s="88">
-        <v>100</v>
-      </c>
-      <c r="E54" s="71"/>
-      <c r="F54" s="71"/>
-      <c r="G54" s="88" t="s">
-        <v>49</v>
-      </c>
-      <c r="H54" s="86" t="s">
-        <v>154</v>
-      </c>
-      <c r="I54" s="88" t="s">
-        <v>259</v>
-      </c>
-      <c r="J54" s="71"/>
-      <c r="K54" s="71"/>
-    </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A55" s="87" t="s">
-        <v>258</v>
-      </c>
-      <c r="B55" s="71"/>
-      <c r="C55" s="87" t="s">
-        <v>63</v>
-      </c>
-      <c r="D55" s="88">
-        <v>200</v>
-      </c>
-      <c r="E55" s="71"/>
-      <c r="F55" s="71"/>
-      <c r="G55" s="88" t="s">
-        <v>49</v>
-      </c>
-      <c r="H55" s="86" t="s">
-        <v>154</v>
-      </c>
-      <c r="I55" s="88" t="s">
-        <v>260</v>
-      </c>
-      <c r="J55" s="71"/>
-      <c r="K55" s="71"/>
-    </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A56" s="87" t="s">
-        <v>261</v>
-      </c>
-      <c r="B56" s="71"/>
-      <c r="C56" s="87" t="s">
-        <v>63</v>
-      </c>
-      <c r="D56" s="88">
-        <v>100</v>
-      </c>
-      <c r="E56" s="71"/>
-      <c r="F56" s="71"/>
-      <c r="G56" s="88" t="s">
-        <v>49</v>
-      </c>
-      <c r="H56" s="71" t="s">
-        <v>50</v>
-      </c>
-      <c r="I56" s="88" t="s">
-        <v>261</v>
-      </c>
-      <c r="J56" s="71"/>
-      <c r="K56" s="71"/>
-    </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A57" s="89" t="s">
-        <v>262</v>
-      </c>
-      <c r="C57" s="87" t="s">
-        <v>63</v>
-      </c>
-      <c r="D57" s="88">
-        <v>3</v>
-      </c>
-      <c r="E57" s="88" t="s">
-        <v>93</v>
-      </c>
-      <c r="G57" s="88" t="s">
-        <v>49</v>
-      </c>
-      <c r="H57" s="75" t="s">
-        <v>263</v>
-      </c>
-      <c r="I57" s="90" t="s">
-        <v>262</v>
-      </c>
-      <c r="K57" s="91" t="s">
-        <v>264</v>
+      <c r="D48" s="102">
+        <v>4000</v>
+      </c>
+      <c r="E48" s="102"/>
+      <c r="F48" s="102"/>
+      <c r="G48" s="102" t="s">
+        <v>49</v>
+      </c>
+      <c r="H48" s="103" t="s">
+        <v>343</v>
+      </c>
+      <c r="I48" s="103" t="s">
+        <v>314</v>
+      </c>
+      <c r="J48" s="102"/>
+      <c r="K48" s="103" t="s">
+        <v>345</v>
       </c>
     </row>
   </sheetData>
@@ -6745,7 +6720,7 @@
   <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6763,7 +6738,7 @@
         <v>17</v>
       </c>
       <c r="B1" s="28" t="s">
-        <v>291</v>
+        <v>351</v>
       </c>
       <c r="C1" s="27"/>
       <c r="D1" s="27"/>
@@ -6797,7 +6772,7 @@
         <v>19</v>
       </c>
       <c r="B3" s="27" t="s">
-        <v>292</v>
+        <v>351</v>
       </c>
       <c r="C3" s="27"/>
       <c r="D3" s="27"/>
@@ -6814,7 +6789,7 @@
         <v>20</v>
       </c>
       <c r="B4" s="27" t="s">
-        <v>293</v>
+        <v>354</v>
       </c>
       <c r="C4" s="27"/>
       <c r="D4" s="27"/>
@@ -6909,65 +6884,65 @@
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="94" t="s">
-        <v>294</v>
-      </c>
-      <c r="B9" s="95"/>
-      <c r="C9" s="95" t="s">
+      <c r="A9" s="84" t="s">
+        <v>287</v>
+      </c>
+      <c r="B9" s="85"/>
+      <c r="C9" s="85" t="s">
         <v>62</v>
       </c>
-      <c r="D9" s="95"/>
-      <c r="E9" s="95"/>
-      <c r="F9" s="95"/>
-      <c r="G9" s="95"/>
-      <c r="H9" s="95"/>
-      <c r="I9" s="95"/>
-      <c r="J9" s="95"/>
-      <c r="K9" s="95"/>
+      <c r="D9" s="85"/>
+      <c r="E9" s="85"/>
+      <c r="F9" s="85"/>
+      <c r="G9" s="85"/>
+      <c r="H9" s="85"/>
+      <c r="I9" s="85"/>
+      <c r="J9" s="85"/>
+      <c r="K9" s="85"/>
     </row>
     <row r="10" spans="1:11" ht="120" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="95" t="s">
+      <c r="A10" s="85" t="s">
         <v>135</v>
       </c>
-      <c r="B10" s="95"/>
-      <c r="C10" s="95" t="s">
+      <c r="B10" s="85"/>
+      <c r="C10" s="85" t="s">
         <v>62</v>
       </c>
-      <c r="D10" s="95"/>
-      <c r="E10" s="95"/>
-      <c r="F10" s="95"/>
-      <c r="G10" s="95"/>
-      <c r="H10" s="95" t="s">
-        <v>295</v>
-      </c>
-      <c r="I10" s="95" t="s">
+      <c r="D10" s="85"/>
+      <c r="E10" s="85"/>
+      <c r="F10" s="85"/>
+      <c r="G10" s="85"/>
+      <c r="H10" s="85" t="s">
+        <v>288</v>
+      </c>
+      <c r="I10" s="85" t="s">
         <v>135</v>
       </c>
-      <c r="J10" s="95"/>
-      <c r="K10" s="96" t="s">
-        <v>297</v>
+      <c r="J10" s="85"/>
+      <c r="K10" s="86" t="s">
+        <v>290</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="95" t="s">
-        <v>285</v>
-      </c>
-      <c r="B11" s="95"/>
-      <c r="C11" s="95" t="s">
+      <c r="A11" s="85" t="s">
+        <v>281</v>
+      </c>
+      <c r="B11" s="85"/>
+      <c r="C11" s="85" t="s">
         <v>62</v>
       </c>
-      <c r="D11" s="95"/>
-      <c r="E11" s="95"/>
-      <c r="F11" s="95"/>
-      <c r="G11" s="95"/>
-      <c r="H11" s="95" t="s">
-        <v>296</v>
-      </c>
-      <c r="I11" s="95" t="s">
-        <v>285</v>
-      </c>
-      <c r="J11" s="95"/>
-      <c r="K11" s="97"/>
+      <c r="D11" s="85"/>
+      <c r="E11" s="85"/>
+      <c r="F11" s="85"/>
+      <c r="G11" s="85"/>
+      <c r="H11" s="85" t="s">
+        <v>289</v>
+      </c>
+      <c r="I11" s="85" t="s">
+        <v>281</v>
+      </c>
+      <c r="J11" s="85"/>
+      <c r="K11" s="87"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -6985,7 +6960,7 @@
   <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7005,7 +6980,7 @@
         <v>17</v>
       </c>
       <c r="B1" s="28" t="s">
-        <v>281</v>
+        <v>352</v>
       </c>
       <c r="C1" s="27"/>
       <c r="D1" s="27"/>
@@ -7039,7 +7014,7 @@
         <v>19</v>
       </c>
       <c r="B3" s="27" t="s">
-        <v>282</v>
+        <v>352</v>
       </c>
       <c r="C3" s="27"/>
       <c r="D3" s="27"/>
@@ -7056,7 +7031,7 @@
         <v>20</v>
       </c>
       <c r="B4" s="27" t="s">
-        <v>283</v>
+        <v>353</v>
       </c>
       <c r="C4" s="27"/>
       <c r="D4" s="27"/>
@@ -7151,8 +7126,8 @@
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="93" t="s">
-        <v>284</v>
+      <c r="A9" s="83" t="s">
+        <v>280</v>
       </c>
       <c r="B9" s="71"/>
       <c r="C9" s="71" t="s">
@@ -7168,8 +7143,8 @@
       <c r="K9" s="71"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="93" t="s">
-        <v>285</v>
+      <c r="A10" s="83" t="s">
+        <v>281</v>
       </c>
       <c r="B10" s="71"/>
       <c r="C10" s="71" t="s">
@@ -7182,10 +7157,10 @@
         <v>49</v>
       </c>
       <c r="H10" s="71" t="s">
-        <v>290</v>
-      </c>
-      <c r="I10" s="93" t="s">
-        <v>285</v>
+        <v>286</v>
+      </c>
+      <c r="I10" s="83" t="s">
+        <v>281</v>
       </c>
       <c r="J10" s="71" t="s">
         <v>62</v>
@@ -7193,8 +7168,8 @@
       <c r="K10" s="71"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="93" t="s">
-        <v>286</v>
+      <c r="A11" s="83" t="s">
+        <v>282</v>
       </c>
       <c r="B11" s="71"/>
       <c r="C11" s="71" t="s">
@@ -7209,10 +7184,10 @@
         <v>49</v>
       </c>
       <c r="H11" s="71" t="s">
-        <v>290</v>
-      </c>
-      <c r="I11" s="93" t="s">
         <v>286</v>
+      </c>
+      <c r="I11" s="83" t="s">
+        <v>282</v>
       </c>
       <c r="J11" s="71" t="s">
         <v>63</v>
@@ -7220,15 +7195,15 @@
       <c r="K11" s="71"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="93" t="s">
-        <v>287</v>
+      <c r="A12" s="83" t="s">
+        <v>283</v>
       </c>
       <c r="B12" s="71"/>
       <c r="C12" s="71" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="D12" s="71" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="E12" s="71"/>
       <c r="F12" s="71"/>
@@ -7236,18 +7211,18 @@
         <v>49</v>
       </c>
       <c r="H12" s="71" t="s">
-        <v>290</v>
-      </c>
-      <c r="I12" s="93" t="s">
-        <v>287</v>
+        <v>286</v>
+      </c>
+      <c r="I12" s="83" t="s">
+        <v>283</v>
       </c>
       <c r="J12" s="71" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="K12" s="71"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="92"/>
+      <c r="A13" s="82"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Add wing_dim to RiskMan datamart.
</commit_message>
<xml_diff>
--- a/Matrix_Bus/RiskMan Bus Matrix.xlsx
+++ b/Matrix_Bus/RiskMan Bus Matrix.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Frank\source\Report\Matrix_Bus\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="7050" windowWidth="24090" windowHeight="3075" activeTab="5"/>
+    <workbookView xWindow="-90" yWindow="7050" windowWidth="24090" windowHeight="3075" firstSheet="11" activeTab="16"/>
   </bookViews>
   <sheets>
     <sheet name="Bus Matrix" sheetId="1" r:id="rId1"/>
@@ -23,15 +28,16 @@
     <sheet name="Program_DIM" sheetId="11" r:id="rId14"/>
     <sheet name="Incident_Type_DIM" sheetId="13" r:id="rId15"/>
     <sheet name="action_dim" sheetId="15" r:id="rId16"/>
-    <sheet name="incident_type_fact" sheetId="14" r:id="rId17"/>
-    <sheet name="incident_action_fact" sheetId="16" r:id="rId18"/>
+    <sheet name="wing_dim" sheetId="23" r:id="rId17"/>
+    <sheet name="incident_type_fact" sheetId="14" r:id="rId18"/>
+    <sheet name="incident_action_fact" sheetId="16" r:id="rId19"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1240" uniqueCount="368">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1279" uniqueCount="378">
   <si>
     <t>Category</t>
   </si>
@@ -1173,12 +1179,42 @@
   <si>
     <t>vwReg_RMFeedback.FBIssuePrevRECID=vwSF_FBIssue.Keydata</t>
   </si>
+  <si>
+    <t>Wing</t>
+  </si>
+  <si>
+    <t>WING_DIM</t>
+  </si>
+  <si>
+    <t>Locating field used for locating events in Riskman system</t>
+  </si>
+  <si>
+    <t>This dim defines all posible locations for one site.</t>
+  </si>
+  <si>
+    <t>[ANGCARE_ID]</t>
+  </si>
+  <si>
+    <t>Key in Riskman system</t>
+  </si>
+  <si>
+    <t>[Wing]</t>
+  </si>
+  <si>
+    <t>The name of wing</t>
+  </si>
+  <si>
+    <t>[ANGCARE_IFR]</t>
+  </si>
+  <si>
+    <t>wing_key</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="13" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1264,6 +1300,14 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -1297,7 +1341,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="28">
+  <borders count="29">
     <border>
       <left/>
       <right/>
@@ -1646,11 +1690,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="128">
+  <cellXfs count="130">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -1893,8 +1949,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="28" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="45"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1902,6 +1965,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1950,7 +2016,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1985,7 +2051,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2197,7 +2263,7 @@
   <dimension ref="A1:V8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L15" sqref="L15"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2233,7 +2299,7 @@
       <c r="U1" s="36"/>
       <c r="V1" s="2"/>
     </row>
-    <row r="2" spans="1:22" ht="86.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:22" ht="87" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -2280,10 +2346,12 @@
       <c r="P2" s="37" t="s">
         <v>16</v>
       </c>
-      <c r="Q2" s="37" t="s">
+      <c r="Q2" s="128" t="s">
         <v>252</v>
       </c>
-      <c r="R2"/>
+      <c r="R2" s="129" t="s">
+        <v>368</v>
+      </c>
       <c r="V2" s="2"/>
     </row>
     <row r="3" spans="1:22" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -2326,7 +2394,7 @@
       <c r="O3" s="63"/>
       <c r="P3" s="62"/>
       <c r="Q3" s="62"/>
-      <c r="R3"/>
+      <c r="R3" s="62"/>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" s="57" t="s">
@@ -2355,7 +2423,7 @@
       <c r="N4" s="65"/>
       <c r="O4" s="65"/>
       <c r="Q4" s="38"/>
-      <c r="R4"/>
+      <c r="R4" s="38"/>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" s="57" t="s">
@@ -2383,7 +2451,7 @@
       <c r="Q5" s="66" t="s">
         <v>4</v>
       </c>
-      <c r="R5"/>
+      <c r="R5" s="66"/>
     </row>
     <row r="6" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="57" t="s">
@@ -2411,6 +2479,7 @@
       <c r="O6" s="40"/>
       <c r="P6" s="40"/>
       <c r="Q6" s="40"/>
+      <c r="R6" s="40"/>
     </row>
     <row r="7" spans="1:22" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="D7" s="38"/>
@@ -2427,6 +2496,7 @@
       <c r="O7" s="38"/>
       <c r="P7" s="38"/>
       <c r="Q7" s="38"/>
+      <c r="R7" s="38"/>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A8" s="43" t="s">
@@ -2472,8 +2542,13 @@
         <v>4</v>
       </c>
       <c r="Q8" s="38"/>
+      <c r="R8" s="38"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="Q2" location="action_dim!A1" display="Action"/>
+    <hyperlink ref="R2" location="wing_dim!A1" display="Wing"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
@@ -3394,7 +3469,7 @@
   <dimension ref="A1:K19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A16:XFD16"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3793,6 +3868,201 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I20" sqref="I20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="38.5703125" style="27" customWidth="1"/>
+    <col min="2" max="2" width="64.28515625" style="27" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="9.140625" style="27"/>
+    <col min="5" max="5" width="15.140625" style="27" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" style="27"/>
+    <col min="7" max="7" width="14" style="27" customWidth="1"/>
+    <col min="8" max="8" width="14.85546875" style="27" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.85546875" style="27" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.5703125" style="27" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="66.5703125" style="27" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="27"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A1" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="28" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="30" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="27" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="27" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="30" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="27" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="27" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="27" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="F8" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="G8" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="H8" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="I8" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="J8" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="K8" s="12" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="17" t="s">
+        <v>377</v>
+      </c>
+      <c r="B9" s="103" t="s">
+        <v>48</v>
+      </c>
+      <c r="C9" s="103" t="s">
+        <v>62</v>
+      </c>
+      <c r="D9" s="103"/>
+      <c r="E9" s="103"/>
+      <c r="F9" s="103"/>
+      <c r="G9" s="103"/>
+      <c r="H9" s="103"/>
+      <c r="I9" s="103"/>
+      <c r="J9" s="103"/>
+      <c r="K9" s="103"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="22" t="s">
+        <v>372</v>
+      </c>
+      <c r="B10" s="103" t="s">
+        <v>373</v>
+      </c>
+      <c r="C10" s="103" t="s">
+        <v>62</v>
+      </c>
+      <c r="D10" s="103"/>
+      <c r="E10" s="103"/>
+      <c r="F10" s="103"/>
+      <c r="G10" s="103" t="s">
+        <v>49</v>
+      </c>
+      <c r="H10" s="103" t="s">
+        <v>376</v>
+      </c>
+      <c r="I10" s="103" t="s">
+        <v>372</v>
+      </c>
+      <c r="J10" s="103"/>
+      <c r="K10" s="45"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="22" t="s">
+        <v>374</v>
+      </c>
+      <c r="B11" s="103" t="s">
+        <v>375</v>
+      </c>
+      <c r="C11" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="D11" s="103">
+        <v>100</v>
+      </c>
+      <c r="E11" s="103"/>
+      <c r="F11" s="103"/>
+      <c r="G11" s="103" t="s">
+        <v>49</v>
+      </c>
+      <c r="H11" s="103" t="s">
+        <v>376</v>
+      </c>
+      <c r="I11" s="103" t="s">
+        <v>374</v>
+      </c>
+      <c r="J11" s="103"/>
+      <c r="K11" s="45"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="103"/>
+      <c r="B12" s="103"/>
+      <c r="C12" s="103"/>
+      <c r="D12" s="103"/>
+      <c r="E12" s="103"/>
+      <c r="F12" s="103"/>
+      <c r="G12" s="103"/>
+      <c r="H12" s="103"/>
+      <c r="I12" s="103"/>
+      <c r="J12" s="103"/>
+      <c r="K12" s="103"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K12"/>
   <sheetViews>
@@ -4055,7 +4325,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K12"/>
   <sheetViews>
@@ -7518,7 +7788,7 @@
   </sheetPr>
   <dimension ref="A1:K14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>

</xml_diff>